<commit_message>
Edits to word doc and excel file
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB4D3B5-2BF8-433B-9F75-8A2BC8EBE389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7183ED5B-496D-4089-943E-F970DF143FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="Capacities" sheetId="5" r:id="rId5"/>
     <sheet name="Example1-Credit" sheetId="8" r:id="rId6"/>
     <sheet name="Example2-Debit" sheetId="9" r:id="rId7"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId8"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId9"/>
-    <sheet name="By User" sheetId="2" r:id="rId10"/>
+    <sheet name="BasinConservationProgram" sheetId="11" r:id="rId8"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId9"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId10"/>
+    <sheet name="By User" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="109">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -352,13 +353,56 @@
   </si>
   <si>
     <t>Debits</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Colorado River Conservation Programs</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Compensation ($ per acre-foot)</t>
+  </si>
+  <si>
+    <t>Lake Mead Water Conservation Accounts</t>
+  </si>
+  <si>
+    <t>2007 to present</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Volume conserved (million acre-feet)</t>
+  </si>
+  <si>
+    <t>System Conservation Pilot Program</t>
+  </si>
+  <si>
+    <t>2015 to 2019</t>
+  </si>
+  <si>
+    <t>500+ Plan</t>
+  </si>
+  <si>
+    <t>2021 to 2022</t>
+  </si>
+  <si>
+    <t>$77 to $240</t>
+  </si>
+  <si>
+    <t>Mandatory Conservation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -498,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -550,9 +594,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -564,9 +605,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -577,7 +615,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -954,6 +1013,184 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
+  <dimension ref="A2:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="2">
+        <v>192000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>47434</v>
+      </c>
+      <c r="G3" s="2">
+        <v>133174</v>
+      </c>
+      <c r="H3" s="2">
+        <f>SUM(E3:G3)</f>
+        <v>180608</v>
+      </c>
+      <c r="I3" s="2">
+        <f>D3-H3</f>
+        <v>11392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H5" si="0">SUM(E4:G4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I5" si="1">D4-H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="2">
+        <v>203392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" s="11">
+        <f>SUM(F3:F5)</f>
+        <v>55434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
@@ -2174,7 +2411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C452AE-E84E-4682-A6B7-6BBA39D2CE31}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -2657,18 +2894,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135C6C2E-A96D-4A95-ACC7-907DE46CB0E8}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="11">
         <f>SUM(B4:B20)</f>
         <v>4119935</v>
@@ -2677,8 +2915,12 @@
         <f>SUM(C4:C20)</f>
         <v>791971</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" s="11">
+        <f>B1-C1</f>
+        <v>3327964</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>Deposits!A1</f>
         <v>Year</v>
@@ -2690,7 +2932,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>Deposits!A2</f>
         <v>2007</v>
@@ -2704,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>Deposits!A3</f>
         <v>2008</v>
@@ -2718,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>Deposits!A4</f>
         <v>2009</v>
@@ -2732,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>Deposits!A5</f>
         <v>2010</v>
@@ -2746,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>Deposits!A6</f>
         <v>2011</v>
@@ -2760,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>Deposits!A7</f>
         <v>2012</v>
@@ -2774,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>Deposits!A8</f>
         <v>2013</v>
@@ -2788,7 +3030,7 @@
         <v>105723</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>Deposits!A9</f>
         <v>2014</v>
@@ -2802,7 +3044,7 @@
         <v>304978</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>Deposits!A10</f>
         <v>2015</v>
@@ -2816,7 +3058,7 @@
         <v>125036</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>Deposits!A11</f>
         <v>2016</v>
@@ -2830,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>Deposits!A12</f>
         <v>2017</v>
@@ -2844,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>Deposits!A13</f>
         <v>2018</v>
@@ -2858,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <f>Deposits!A14</f>
         <v>2019</v>
@@ -3132,14 +3374,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -3218,86 +3460,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>2700000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:3" s="23" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <f>Balances!B12</f>
         <v>126800</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <f>C5-C8</f>
         <v>2483748</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <f>Deposits!C13</f>
         <v>216252</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <f>C6+C8</f>
         <v>343052</v>
       </c>
@@ -3327,91 +3569,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>4400000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:3" s="23" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <f>Balances!C16</f>
         <v>1357085</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <f>C5 + ABS(Deposits!D17)</f>
         <v>4511392</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <f>C7-C5</f>
         <v>111392</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <f>C6-C8</f>
         <v>1245693</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
+      <c r="A10" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3422,6 +3664,112 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B9E5BA-6A58-4021-B418-75CB2886B06A}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.26953125" customWidth="1"/>
+    <col min="2" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="40">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="40">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="41">
+        <v>200</v>
+      </c>
+      <c r="D6" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="22">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="40">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -3437,11 +3785,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -3697,147 +4045,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
-  <dimension ref="A2:I7"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="2">
-        <v>192000</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>47434</v>
-      </c>
-      <c r="G3" s="2">
-        <v>133174</v>
-      </c>
-      <c r="H3" s="2">
-        <f>SUM(E3:G3)</f>
-        <v>180608</v>
-      </c>
-      <c r="I3" s="2">
-        <f>D3-H3</f>
-        <v>11392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>2020</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H5" si="0">SUM(E4:G4)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" ref="I4:I5" si="1">D4-H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5">
-        <v>2020</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8000</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8000</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F7" s="11">
-        <f>SUM(F3:F5)</f>
-        <v>55434</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Edits to Word file and table of Colorado River basin conservation program accomplishements
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7183ED5B-496D-4089-943E-F970DF143FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1917EC-6B70-4D79-A057-B75B89CD8DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -370,42 +370,64 @@
     <t>Lake Mead Water Conservation Accounts</t>
   </si>
   <si>
-    <t>2007 to present</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t>Volume conserved (million acre-feet)</t>
-  </si>
-  <si>
-    <t>System Conservation Pilot Program</t>
-  </si>
-  <si>
     <t>2015 to 2019</t>
   </si>
   <si>
-    <t>500+ Plan</t>
-  </si>
-  <si>
     <t>2021 to 2022</t>
   </si>
   <si>
     <t>$77 to $240</t>
   </si>
   <si>
-    <t>Mandatory Conservation</t>
+    <t>$150 to $611</t>
+  </si>
+  <si>
+    <t>2015 to 2017</t>
+  </si>
+  <si>
+    <t>$161 to $670</t>
+  </si>
+  <si>
+    <t>2019 to 2023</t>
+  </si>
+  <si>
+    <t>Mandatory Conservation - Not ICS</t>
+  </si>
+  <si>
+    <t>500+ Plan - Lower Basin</t>
+  </si>
+  <si>
+    <t>Compensation ($ million)</t>
+  </si>
+  <si>
+    <t>Volume (million acre-feet)</t>
+  </si>
+  <si>
+    <t>2007 to 2023</t>
+  </si>
+  <si>
+    <t>System Conservation Pilot Programs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lower Basin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Upper Basin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -542,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -591,9 +613,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -625,17 +644,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,21 +1048,30 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
-  <dimension ref="A2:I8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G1" s="11">
+        <f>SUM(G3:G14)</f>
+        <v>631210</v>
+      </c>
+    </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
@@ -1157,6 +1200,15 @@
       <c r="D6" s="2">
         <v>203392</v>
       </c>
+      <c r="F6" s="2">
+        <v>48296</v>
+      </c>
+      <c r="G6" s="2">
+        <v>155096</v>
+      </c>
+      <c r="H6">
+        <v>203392</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1165,10 +1217,11 @@
       <c r="C7">
         <v>2021</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
       <c r="F7" s="11">
-        <f>SUM(F3:F5)</f>
-        <v>55434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1183,6 +1236,117 @@
       </c>
       <c r="D8" s="2">
         <v>8000</v>
+      </c>
+      <c r="F8" s="11">
+        <v>8000</v>
+      </c>
+      <c r="H8" s="11">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="2">
+        <v>192000</v>
+      </c>
+      <c r="F9">
+        <v>57061</v>
+      </c>
+      <c r="G9">
+        <v>134940</v>
+      </c>
+      <c r="H9">
+        <f>SUM(E9:G9)</f>
+        <v>192001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G10">
+        <v>8000</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H14" si="2">SUM(E10:G10)</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="2">
+        <v>192000</v>
+      </c>
+      <c r="G12">
+        <v>192000</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>192000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>2023</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G13">
+        <v>8000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2023</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3374,14 +3538,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -3460,86 +3624,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>2700000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="23" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:3" s="22" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <f>Balances!B12</f>
         <v>126800</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <f>C5-C8</f>
         <v>2483748</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <f>Deposits!C13</f>
         <v>216252</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f>C6+C8</f>
         <v>343052</v>
       </c>
@@ -3569,91 +3733,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>4400000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="23" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:3" s="22" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <f>Balances!C16</f>
         <v>1357085</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <f>C5 + ABS(Deposits!D17)</f>
         <v>4511392</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <f>C7-C5</f>
         <v>111392</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f>C6-C8</f>
         <v>1245693</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="34"/>
+      <c r="A10" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3665,106 +3829,162 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B9E5BA-6A58-4021-B418-75CB2886B06A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
-    <col min="2" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="E3" s="41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="37">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="39">
+        <v>200</v>
+      </c>
+      <c r="E5" s="44">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="37">
+        <f>DCPLogs!G1/1000000</f>
+        <v>0.63121000000000005</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="E6" s="45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="40">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="C8" s="37">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="D8" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="E8" s="44">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="38">
+        <v>2023</v>
+      </c>
+      <c r="C9" s="37">
+        <f>(2517+4633+15091+15571)/1000000</f>
+        <v>3.7811999999999998E-2</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="E9" s="44">
+        <f>0.992+1.205+5.344+8.335</f>
+        <v>15.876000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="C10" s="37">
+        <v>2.2116E-2</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="41">
-        <v>200</v>
-      </c>
-      <c r="D6" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="22">
-        <v>2023</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="40">
-        <v>4.2999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="5"/>
+      <c r="E10" s="44">
+        <v>4.5599999999999996</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E10">
+    <sortCondition descending="1" ref="C4:C10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3785,11 +4005,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">

</xml_diff>

<commit_message>
Updates to word doc and excel file
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1917EC-6B70-4D79-A057-B75B89CD8DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C56C4E2-7178-4E4D-88A6-F044B5EB55AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
     <sheet name="Balances" sheetId="1" r:id="rId2"/>
     <sheet name="Deposits" sheetId="7" r:id="rId3"/>
-    <sheet name="TotalDepositsCredits" sheetId="10" r:id="rId4"/>
+    <sheet name="TotalCreditsDebits" sheetId="10" r:id="rId4"/>
     <sheet name="Capacities" sheetId="5" r:id="rId5"/>
     <sheet name="Example1-Credit" sheetId="8" r:id="rId6"/>
     <sheet name="Example2-Debit" sheetId="9" r:id="rId7"/>
-    <sheet name="BasinConservationProgram" sheetId="11" r:id="rId8"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId9"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId10"/>
-    <sheet name="By User" sheetId="2" r:id="rId11"/>
+    <sheet name="BasinConservationPrograms" sheetId="11" r:id="rId8"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId9"/>
+    <sheet name="By User" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -187,30 +186,6 @@
     <t>Balance - Dec 2019 (AF)</t>
   </si>
   <si>
-    <t>DCP-AZ Reduction (ac-ft)</t>
-  </si>
-  <si>
-    <t>DCP-NV Reduction (ac-ft)</t>
-  </si>
-  <si>
-    <t>DCP-CA Reduction (ac-ft)</t>
-  </si>
-  <si>
-    <t>Mead Elevation (ft)</t>
-  </si>
-  <si>
-    <t>Years ICS can convert to DCP</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>NV</t>
-  </si>
-  <si>
     <t>Balance - Dec 2020 (AF)</t>
   </si>
   <si>
@@ -268,9 +243,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>1. Balances</t>
-  </si>
-  <si>
     <t>Water Conservation account balances, credits, and debits, by year and entity.</t>
   </si>
   <si>
@@ -280,27 +252,9 @@
     <t>Explanation of how users met drought contingency plan (DPC) required conservation.</t>
   </si>
   <si>
-    <t>Number of years state can use ICS balance to meet drought contingency plan (DCP) required conservation</t>
-  </si>
-  <si>
-    <t>2. Deposits</t>
-  </si>
-  <si>
     <t>Annual deposits and withdraws calculated as the year to year difference in balances.</t>
   </si>
   <si>
-    <t>3. Capacities</t>
-  </si>
-  <si>
-    <t>4. ICStoDPC</t>
-  </si>
-  <si>
-    <t>5. DCPLogs</t>
-  </si>
-  <si>
-    <t>6. ByUser</t>
-  </si>
-  <si>
     <t>Account balance by state and contractor</t>
   </si>
   <si>
@@ -416,18 +370,56 @@
   </si>
   <si>
     <t xml:space="preserve">    Upper Basin</t>
+  </si>
+  <si>
+    <t>Example of water conservation program credit using Arizona in 2018</t>
+  </si>
+  <si>
+    <t>Example of water conservation program debit using California in 2022.</t>
+  </si>
+  <si>
+    <t>Balances</t>
+  </si>
+  <si>
+    <t>Deposits</t>
+  </si>
+  <si>
+    <t>Capacities</t>
+  </si>
+  <si>
+    <t>Example1-Credit</t>
+  </si>
+  <si>
+    <t>Example2-Debit</t>
+  </si>
+  <si>
+    <t>DCPLogs</t>
+  </si>
+  <si>
+    <t>ByUser</t>
+  </si>
+  <si>
+    <t>TotalCreditsDebits</t>
+  </si>
+  <si>
+    <t>Sum of all water conservation program credits and debits each year, plus total over all years</t>
+  </si>
+  <si>
+    <t>BasinConservationPrograms</t>
+  </si>
+  <si>
+    <t>Summary of water conserved by each Colorado River Basin conservation program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -466,7 +458,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,18 +473,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -510,15 +496,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -564,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -590,13 +567,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,7 +576,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -626,24 +596,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -665,11 +626,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -952,93 +916,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="46.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>66</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>71</v>
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>73</v>
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>74</v>
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>75</v>
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>76</v>
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1047,318 +1065,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
-  <dimension ref="A1:I14"/>
-  <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9:H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G1" s="11">
-        <f>SUM(G3:G14)</f>
-        <v>631210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="2">
-        <v>192000</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>47434</v>
-      </c>
-      <c r="G3" s="2">
-        <v>133174</v>
-      </c>
-      <c r="H3" s="2">
-        <f>SUM(E3:G3)</f>
-        <v>180608</v>
-      </c>
-      <c r="I3" s="2">
-        <f>D3-H3</f>
-        <v>11392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>2020</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H5" si="0">SUM(E4:G4)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" ref="I4:I5" si="1">D4-H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5">
-        <v>2020</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8000</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8000</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6">
-        <v>2021</v>
-      </c>
-      <c r="D6" s="2">
-        <v>203392</v>
-      </c>
-      <c r="F6" s="2">
-        <v>48296</v>
-      </c>
-      <c r="G6" s="2">
-        <v>155096</v>
-      </c>
-      <c r="H6">
-        <v>203392</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2021</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8">
-        <v>2021</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8000</v>
-      </c>
-      <c r="F8" s="11">
-        <v>8000</v>
-      </c>
-      <c r="H8" s="11">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="2">
-        <v>192000</v>
-      </c>
-      <c r="F9">
-        <v>57061</v>
-      </c>
-      <c r="G9">
-        <v>134940</v>
-      </c>
-      <c r="H9">
-        <f>SUM(E9:G9)</f>
-        <v>192001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>2022</v>
-      </c>
-      <c r="D10" s="2">
-        <v>8000</v>
-      </c>
-      <c r="G10">
-        <v>8000</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H14" si="2">SUM(E10:G10)</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>2022</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>2023</v>
-      </c>
-      <c r="D12" s="2">
-        <v>192000</v>
-      </c>
-      <c r="G12">
-        <v>192000</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>192000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>2023</v>
-      </c>
-      <c r="D13" s="2">
-        <v>8000</v>
-      </c>
-      <c r="G13">
-        <v>8000</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>2023</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
@@ -2034,7 +1744,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -2043,12 +1753,12 @@
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -2076,7 +1786,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2">
         <v>100000</v>
@@ -2105,7 +1815,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2">
         <v>100000</v>
@@ -2449,18 +2159,18 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="16">
+        <v>39</v>
+      </c>
+      <c r="B15" s="13">
         <v>598742</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>1375871</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>865741</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <f>E14+41000</f>
         <v>173975</v>
       </c>
@@ -2468,7 +2178,7 @@
         <f t="shared" si="1"/>
         <v>2840354</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="14">
         <v>2020</v>
       </c>
       <c r="H15" s="11">
@@ -2478,18 +2188,18 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="16">
+        <v>49</v>
+      </c>
+      <c r="B16" s="13">
         <v>684201</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>1357085</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>949658</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <f>E15+41000</f>
         <v>214975</v>
       </c>
@@ -2497,7 +2207,7 @@
         <f t="shared" si="1"/>
         <v>2990944</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="14">
         <v>2021</v>
       </c>
       <c r="H16" s="11">
@@ -2507,18 +2217,18 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="16">
+        <v>50</v>
+      </c>
+      <c r="B17" s="13">
         <v>753423</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="13">
         <v>1245693</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>1038765</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <f>30000+E16</f>
         <v>244975</v>
       </c>
@@ -2526,7 +2236,7 @@
         <f t="shared" si="1"/>
         <v>3037881</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="14">
         <v>2022</v>
       </c>
       <c r="H17" s="11">
@@ -2536,18 +2246,18 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="21">
+        <v>51</v>
+      </c>
+      <c r="B18" s="18">
         <v>710589</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="18">
         <v>1661832</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="18">
         <v>955543</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="15">
         <f>E17-34000</f>
         <v>210975</v>
       </c>
@@ -2589,24 +2299,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="str" cm="1">
+      <c r="A1" s="17" t="str" cm="1">
         <f t="array" ref="A1">Balances!G1:G1</f>
         <v>Year</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>48</v>
+      <c r="F1" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2614,23 +2324,23 @@
         <f>Balances!G2</f>
         <v>2007</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="13">
         <f>SUM(C2:F2)</f>
         <v>41398</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <f>Balances!B2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <f>Balances!C2</f>
         <v>41398</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="13">
         <f>Balances!D2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="13">
         <f>Balances!E3-Balances!E2</f>
         <v>0</v>
       </c>
@@ -2640,23 +2350,23 @@
         <f>Balances!G3</f>
         <v>2008</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="13">
         <f t="shared" ref="B3:B18" si="0">SUM(C3:F3)</f>
         <v>552175</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <f>Balances!B3-Balances!B2</f>
         <v>100000</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <f>Balances!C3-Balances!C2</f>
         <v>52175</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <f>Balances!D3-Balances!D2</f>
         <v>400000</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <f>Balances!E3-Balances!E2</f>
         <v>0</v>
       </c>
@@ -2666,23 +2376,23 @@
         <f>Balances!G4</f>
         <v>2009</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <f t="shared" si="0"/>
         <v>63617</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <f>Balances!B4-Balances!B3</f>
         <v>0</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <f>Balances!C4-Balances!C3</f>
         <v>63617</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <f>Balances!D4-Balances!D3</f>
         <v>0</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <f>Balances!E4-Balances!E3</f>
         <v>0</v>
       </c>
@@ -2692,23 +2402,23 @@
         <f>Balances!G5</f>
         <v>2010</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="13">
         <f t="shared" si="0"/>
         <v>158151</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <f>Balances!B5-Balances!B4</f>
         <v>2094</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <f>Balances!C5-Balances!C4</f>
         <v>104800</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <f>Balances!D5-Balances!D4</f>
         <v>51257</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <f>Balances!E5-Balances!E4</f>
         <v>0</v>
       </c>
@@ -2718,23 +2428,23 @@
         <f>Balances!G6</f>
         <v>2011</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="13">
         <f t="shared" si="0"/>
         <v>211059</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <f>Balances!B6-Balances!B5</f>
         <v>956</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <f>Balances!C6-Balances!C5</f>
         <v>178688</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <f>Balances!D6-Balances!D5</f>
         <v>31415</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <f>Balances!E6-Balances!E5</f>
         <v>0</v>
       </c>
@@ -2744,23 +2454,23 @@
         <f>Balances!G7</f>
         <v>2012</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="13">
         <f t="shared" si="0"/>
         <v>169240</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <f>Balances!B7-Balances!B6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <f>Balances!C7-Balances!C6</f>
         <v>139108</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <f>Balances!D7-Balances!D6</f>
         <v>30132</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <f>Balances!E7-Balances!E6</f>
         <v>0</v>
       </c>
@@ -2770,23 +2480,23 @@
         <f>Balances!G8</f>
         <v>2013</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="13">
         <f t="shared" si="0"/>
         <v>-77476</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <f>Balances!B8-Balances!B7</f>
         <v>0</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <f>Balances!C8-Balances!C7</f>
         <v>-105723</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <f>Balances!D8-Balances!D7</f>
         <v>28247</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="13">
         <f>Balances!E8-Balances!E7</f>
         <v>0</v>
       </c>
@@ -2796,23 +2506,23 @@
         <f>Balances!G9</f>
         <v>2014</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <f t="shared" si="0"/>
         <v>-281264</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <f>Balances!B9-Balances!B8</f>
         <v>0</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <f>Balances!C9-Balances!C8</f>
         <v>-304978</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <f>Balances!D9-Balances!D8</f>
         <v>23714</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="13">
         <f>Balances!E9-Balances!E8</f>
         <v>0</v>
       </c>
@@ -2822,23 +2532,23 @@
         <f>Balances!G10</f>
         <v>2015</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="13">
         <f t="shared" si="0"/>
         <v>-125036</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <f>Balances!B10-Balances!B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <f>Balances!C10-Balances!C9</f>
         <v>-71294</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <f>Balances!D10-Balances!D9</f>
         <v>-53742</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="13">
         <f>Balances!E10-Balances!E9</f>
         <v>0</v>
       </c>
@@ -2848,23 +2558,23 @@
         <f>Balances!G11</f>
         <v>2016</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <f t="shared" si="0"/>
         <v>37814</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <f>Balances!B11-Balances!B10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <f>Balances!C11-Balances!C10</f>
         <v>17275</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <f>Balances!D11-Balances!D10</f>
         <v>20539</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <f>Balances!E11-Balances!E10</f>
         <v>0</v>
       </c>
@@ -2874,23 +2584,23 @@
         <f>Balances!G12</f>
         <v>2017</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="13">
         <f t="shared" si="0"/>
         <v>511813</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <f>Balances!B12-Balances!B11</f>
         <v>23750</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <f>Balances!C12-Balances!C11</f>
         <v>437312</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <f>Balances!D12-Balances!D11</f>
         <v>50751</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="13">
         <f>Balances!E12-Balances!E11</f>
         <v>0</v>
       </c>
@@ -2900,23 +2610,23 @@
         <f>Balances!G13</f>
         <v>2018</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="13">
         <f t="shared" si="0"/>
         <v>480441</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <f>Balances!B13-Balances!B12</f>
         <v>216252</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <f>Balances!C13-Balances!C12</f>
         <v>146054</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <f>Balances!D13-Balances!D12</f>
         <v>118135</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="13">
         <f>Balances!E13-Balances!E12</f>
         <v>0</v>
       </c>
@@ -2926,23 +2636,23 @@
         <f>Balances!G14</f>
         <v>2019</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="13">
         <f t="shared" si="0"/>
         <v>703670</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <f>Balances!B14-Balances!B13</f>
         <v>130452</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <f>Balances!C14-Balances!C13</f>
         <v>354778</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="13">
         <f>Balances!D14-Balances!D13</f>
         <v>85465</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="13">
         <f>Balances!E14-Balances!E13</f>
         <v>132975</v>
       </c>
@@ -2952,23 +2662,23 @@
         <f>Balances!G15</f>
         <v>2020</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <f t="shared" si="0"/>
         <v>568727</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <f>Balances!B15-Balances!B14</f>
         <v>125238</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <f>Balances!C15-Balances!C14</f>
         <v>322661</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <f>Balances!D15-Balances!D14</f>
         <v>79828</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="13">
         <f>Balances!E15-Balances!E14</f>
         <v>41000</v>
       </c>
@@ -2978,23 +2688,23 @@
         <f>Balances!G16</f>
         <v>2021</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="13">
         <f t="shared" si="0"/>
         <v>191590</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <f>Balances!B16-Balances!B15</f>
         <v>85459</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <f>Balances!C16-Balances!C15</f>
         <v>-18786</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <f>Balances!D16-Balances!D15</f>
         <v>83917</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="13">
         <f>Balances!E16-Balances!E15</f>
         <v>41000</v>
       </c>
@@ -3004,23 +2714,23 @@
         <f>Balances!G17</f>
         <v>2022</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="13">
         <f t="shared" si="0"/>
         <v>76937</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="13">
         <f>Balances!B17-Balances!B16</f>
         <v>69222</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <f>Balances!C17-Balances!C16</f>
         <v>-111392</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <f>Balances!D17-Balances!D16</f>
         <v>89107</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="13">
         <f>Balances!E17-Balances!E16</f>
         <v>30000</v>
       </c>
@@ -3030,23 +2740,23 @@
         <f>Balances!G18</f>
         <v>2023</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="13">
         <f t="shared" si="0"/>
         <v>256083</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <f>Balances!B18-Balances!B17</f>
         <v>-42834</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <f>Balances!C18-Balances!C17</f>
         <v>416139</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <f>Balances!D18-Balances!D17</f>
         <v>-83222</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="13">
         <f>Balances!E18-Balances!E17</f>
         <v>-34000</v>
       </c>
@@ -3089,11 +2799,11 @@
         <f>Deposits!A1</f>
         <v>Year</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>94</v>
+      <c r="B3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3372,7 +3082,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -3538,14 +3248,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -3624,86 +3334,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="23"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="28" t="s">
-        <v>78</v>
+      <c r="B4" s="40"/>
+      <c r="C4" s="25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="25">
+      <c r="A5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22">
         <v>2700000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="22" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="26">
+    <row r="6" spans="1:3" s="19" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="23">
         <f>Balances!B12</f>
         <v>126800</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="25">
+      <c r="A7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="22">
         <f>C5-C8</f>
         <v>2483748</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="25">
+      <c r="A8" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="22">
         <f>Deposits!C13</f>
         <v>216252</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="27">
+      <c r="A9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="24">
         <f>C6+C8</f>
         <v>343052</v>
       </c>
@@ -3733,91 +3443,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="23"/>
+      <c r="A1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="28" t="s">
-        <v>78</v>
+      <c r="B4" s="40"/>
+      <c r="C4" s="25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="25">
+      <c r="A5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22">
         <v>4400000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="22" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="26">
+    <row r="6" spans="1:3" s="19" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="23">
         <f>Balances!C16</f>
         <v>1357085</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="25">
+      <c r="A7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="22">
         <f>C5 + ABS(Deposits!D17)</f>
         <v>4511392</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="25">
+      <c r="A8" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="22">
         <f>C7-C5</f>
         <v>111392</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="27">
+      <c r="A9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="24">
         <f>C6-C8</f>
         <v>1245693</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
+      <c r="A10" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3831,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B9E5BA-6A58-4021-B418-75CB2886B06A}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E10"/>
+    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3846,138 +3556,138 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="41" t="s">
+    <row r="4" spans="1:5" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="37">
+      <c r="C4" s="31">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="37">
+      <c r="D4" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="31">
         <v>1</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="33">
         <v>200</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="38">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="37">
+    <row r="6" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="31">
         <f>DCPLogs!G1/1000000</f>
         <v>0.63121000000000005</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="38">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="37">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="44">
-        <v>29.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="38">
+      <c r="B9" s="32">
         <v>2023</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="31">
         <f>(2517+4633+15091+15571)/1000000</f>
         <v>3.7811999999999998E-2</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="44">
+      <c r="D9" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="38">
         <f>0.992+1.205+5.344+8.335</f>
         <v>15.876000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="37">
+    <row r="10" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="31">
         <v>2.2116E-2</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="44">
+      <c r="D10" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="38">
         <v>4.5599999999999996</v>
       </c>
     </row>
@@ -3990,279 +3700,309 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1048576"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" s="36" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G1" s="11">
+        <f>SUM(G3:G14)</f>
+        <v>631210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="I2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14">
-        <v>1218.5</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
-        <v>1190</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
-        <v>1150</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>1091</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>1090</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="2">
         <v>192000</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>47434</v>
+      </c>
+      <c r="G3" s="2">
+        <v>133174</v>
+      </c>
+      <c r="H3" s="2">
+        <f>SUM(E3:G3)</f>
+        <v>180608</v>
+      </c>
+      <c r="I3" s="2">
+        <f>D3-H3</f>
+        <v>11392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H5" si="0">SUM(E4:G4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I5" si="1">D4-H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="2">
         <v>8000</v>
       </c>
-      <c r="E7" s="15">
-        <f>Balances!B$5/B7</f>
-        <v>0.53173958333333338</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15">
-        <f>Balances!D$5/D7</f>
-        <v>56.407125000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>1075</v>
-      </c>
-      <c r="B8" s="6">
-        <v>512000</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6">
-        <v>21000</v>
-      </c>
-      <c r="E8" s="15">
-        <f>Balances!B$5/B8</f>
-        <v>0.19940234374999999</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
-        <f>Balances!D$5/D8</f>
-        <v>21.488428571428571</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>1050</v>
-      </c>
-      <c r="B9" s="6">
-        <v>592000</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6">
-        <v>25000</v>
-      </c>
-      <c r="E9" s="15">
-        <f>Balances!B$5/B9</f>
-        <v>0.17245608108108107</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15">
-        <f>Balances!D$5/D9</f>
-        <v>18.050280000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>1045</v>
-      </c>
-      <c r="B10" s="6">
-        <v>640000</v>
-      </c>
-      <c r="C10" s="6">
-        <v>200000</v>
-      </c>
-      <c r="D10" s="6">
-        <v>27000</v>
-      </c>
-      <c r="E10" s="15">
-        <f>Balances!B$5/B10</f>
-        <v>0.15952187500000001</v>
-      </c>
-      <c r="F10" s="15">
-        <f>Balances!C$5/C10</f>
-        <v>1.3099499999999999</v>
-      </c>
-      <c r="G10" s="15">
-        <f>Balances!D$5/D10</f>
-        <v>16.713222222222221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>1040</v>
-      </c>
-      <c r="B11" s="6">
-        <v>640000</v>
-      </c>
-      <c r="C11" s="6">
-        <v>250000</v>
-      </c>
-      <c r="D11" s="6">
-        <v>27000</v>
-      </c>
-      <c r="E11" s="15">
-        <f>Balances!B$5/B11</f>
-        <v>0.15952187500000001</v>
-      </c>
-      <c r="F11" s="15">
-        <f>Balances!C$5/C11</f>
-        <v>1.04796</v>
-      </c>
-      <c r="G11" s="15">
-        <f>Balances!D$5/D11</f>
-        <v>16.713222222222221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>1035</v>
-      </c>
-      <c r="B12" s="6">
-        <v>640000</v>
-      </c>
-      <c r="C12" s="6">
-        <v>300000</v>
-      </c>
-      <c r="D12" s="6">
-        <v>27000</v>
-      </c>
-      <c r="E12" s="15">
-        <f>Balances!B$5/B12</f>
-        <v>0.15952187500000001</v>
-      </c>
-      <c r="F12" s="15">
-        <f>Balances!C$5/C12</f>
-        <v>0.87329999999999997</v>
-      </c>
-      <c r="G12" s="15">
-        <f>Balances!D$5/D12</f>
-        <v>16.713222222222221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>1030</v>
-      </c>
-      <c r="B13" s="6">
-        <v>640000</v>
-      </c>
-      <c r="C13" s="6">
-        <v>350000</v>
-      </c>
-      <c r="D13" s="6">
-        <v>27000</v>
-      </c>
-      <c r="E13" s="15">
-        <f>Balances!B$5/B13</f>
-        <v>0.15952187500000001</v>
-      </c>
-      <c r="F13" s="15">
-        <f>Balances!C$5/C13</f>
-        <v>0.74854285714285718</v>
-      </c>
-      <c r="G13" s="15">
-        <f>Balances!D$5/D13</f>
-        <v>16.713222222222221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>1025</v>
-      </c>
-      <c r="B14" s="6">
-        <v>720000</v>
-      </c>
-      <c r="C14" s="6">
-        <v>350000</v>
-      </c>
-      <c r="D14" s="6">
-        <v>30000</v>
-      </c>
-      <c r="E14" s="15">
-        <f>Balances!B$5/B14</f>
-        <v>0.14179722222222221</v>
-      </c>
-      <c r="F14" s="15">
-        <f>Balances!C$5/C14</f>
-        <v>0.74854285714285718</v>
-      </c>
-      <c r="G14" s="15">
-        <f>Balances!D$5/D14</f>
-        <v>15.0419</v>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="2">
+        <v>203392</v>
+      </c>
+      <c r="F6" s="2">
+        <v>48296</v>
+      </c>
+      <c r="G6" s="2">
+        <v>155096</v>
+      </c>
+      <c r="H6">
+        <v>203392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F8" s="11">
+        <v>8000</v>
+      </c>
+      <c r="H8" s="11">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="2">
+        <v>192000</v>
+      </c>
+      <c r="F9">
+        <v>57061</v>
+      </c>
+      <c r="G9">
+        <v>134940</v>
+      </c>
+      <c r="H9">
+        <f>SUM(E9:G9)</f>
+        <v>192001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G10">
+        <v>8000</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H14" si="2">SUM(E10:G10)</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="2">
+        <v>192000</v>
+      </c>
+      <c r="G12">
+        <v>192000</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>192000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>2023</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G13">
+        <v>8000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2023</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More edits to doc and excel file. Download March 2024 proposals
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C56C4E2-7178-4E4D-88A6-F044B5EB55AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D196E4-33A5-4D82-AC6A-998572A19A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Example2-Debit" sheetId="9" r:id="rId7"/>
     <sheet name="BasinConservationPrograms" sheetId="11" r:id="rId8"/>
     <sheet name="DCPLogs" sheetId="4" r:id="rId9"/>
-    <sheet name="By User" sheetId="2" r:id="rId10"/>
+    <sheet name="AllocateAvailableWater" sheetId="12" r:id="rId10"/>
+    <sheet name="By User" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="125">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -409,17 +410,52 @@
   </si>
   <si>
     <t>Summary of water conserved by each Colorado River Basin conservation program</t>
+  </si>
+  <si>
+    <t>Buschatzke, T., Hamby, J. B., and Entsminger, J. (2024). "Lower Basin Alternative for the Post-2026 Coordinated Operation of the Colorado River Basin." https://www.snwa.com/assets/pdf/lower-basin-alternative-letter-march2024.pdf [Accessed on: August 14, 2024].</t>
+  </si>
+  <si>
+    <t>Use March 2024 Lower Basin Alternative shortages to divide available water among water accounts</t>
+  </si>
+  <si>
+    <t>0.0 to 0.3</t>
+  </si>
+  <si>
+    <t>0.3 to 1.5</t>
+  </si>
+  <si>
+    <t>1.5 to 2.7</t>
+  </si>
+  <si>
+    <t>To be determined</t>
+  </si>
+  <si>
+    <t>Avaliable Water (maf per year) [2]</t>
+  </si>
+  <si>
+    <t>Total Shortage (maf per year) [1]</t>
+  </si>
+  <si>
+    <t>Lower Basin Water Shortages</t>
+  </si>
+  <si>
+    <t>Total Shortage (maf per year)</t>
+  </si>
+  <si>
+    <t>0 (Historical Allocation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -537,11 +573,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -626,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -635,10 +672,39 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -918,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A17"/>
     </sheetView>
   </sheetViews>
@@ -1065,6 +1131,495 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460CD49-F28E-4E8F-9EC7-325148866036}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="44" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0</v>
+      </c>
+      <c r="G8" s="42">
+        <f>SUM(C8:F8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="43">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="E9" s="43">
+        <v>0</v>
+      </c>
+      <c r="F9" s="43">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G9" s="43">
+        <f t="shared" ref="G9:G10" si="0">SUM(C9:F9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="43">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="D10" s="43">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="E10" s="43">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="F10" s="43">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G10" s="43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+    </row>
+    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="46" t="str">
+        <f>B14</f>
+        <v>Avaliable Water (maf per year) [2]</v>
+      </c>
+      <c r="J14" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="50">
+        <f>G15-0</f>
+        <v>9</v>
+      </c>
+      <c r="C15" s="50">
+        <v>2.8</v>
+      </c>
+      <c r="D15" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="50">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F15" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="50">
+        <f>SUM(C15:F15)</f>
+        <v>9</v>
+      </c>
+      <c r="I15" s="47">
+        <f>B15</f>
+        <v>9</v>
+      </c>
+      <c r="J15" s="42">
+        <f>C15/$B15</f>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="K15" s="42">
+        <f t="shared" ref="K15:M15" si="1">D15/$B15</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="L15" s="42">
+        <f t="shared" si="1"/>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="M15" s="42">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N15" s="48">
+        <f>SUM(J15:M15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="B16" s="47">
+        <f>B$15-A16</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C16" s="47">
+        <f>C15-$A16*C9</f>
+        <v>2.5599999999999996</v>
+      </c>
+      <c r="D16" s="47">
+        <f>D15-$A16*D9</f>
+        <v>0.29000999999999999</v>
+      </c>
+      <c r="E16" s="47">
+        <f>E15-$A16*E9</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F16" s="47">
+        <f>F15-$A16*F9</f>
+        <v>1.4499900000000001</v>
+      </c>
+      <c r="G16" s="47">
+        <f t="shared" ref="G16:G20" si="2">SUM(C16:F16)</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I16" s="47">
+        <f>B16</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J16" s="42">
+        <f t="shared" ref="J16:J20" si="3">C16/$B16</f>
+        <v>0.29425287356321839</v>
+      </c>
+      <c r="K16" s="42">
+        <f t="shared" ref="K16:K20" si="4">D16/$B16</f>
+        <v>3.3334482758620693E-2</v>
+      </c>
+      <c r="L16" s="42">
+        <f t="shared" ref="L16:L20" si="5">E16/$B16</f>
+        <v>0.50574712643678166</v>
+      </c>
+      <c r="M16" s="42">
+        <f t="shared" ref="M16:M20" si="6">F16/$B16</f>
+        <v>0.16666551724137935</v>
+      </c>
+      <c r="N16" s="48">
+        <f t="shared" ref="N16:N20" si="7">SUM(J16:M16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="B17" s="47">
+        <f t="shared" ref="B17:B20" si="8">B$15-A17</f>
+        <v>8.6</v>
+      </c>
+      <c r="C17" s="47">
+        <f>C$16-($A17-$A$16)*C$10</f>
+        <v>2.5166699999999995</v>
+      </c>
+      <c r="D17" s="47">
+        <f>D$16-($A17-$A$16)*D$10</f>
+        <v>0.28667999999999999</v>
+      </c>
+      <c r="E17" s="47">
+        <f>E$16-($A17-$A$16)*E$10</f>
+        <v>4.3633300000000004</v>
+      </c>
+      <c r="F17" s="47">
+        <f>F$16-($A17-$A$16)*F$10</f>
+        <v>1.4333200000000001</v>
+      </c>
+      <c r="G17" s="47">
+        <f t="shared" si="2"/>
+        <v>8.6</v>
+      </c>
+      <c r="I17" s="47">
+        <f>B17</f>
+        <v>8.6</v>
+      </c>
+      <c r="J17" s="42">
+        <f t="shared" si="3"/>
+        <v>0.29263604651162789</v>
+      </c>
+      <c r="K17" s="42">
+        <f t="shared" si="4"/>
+        <v>3.3334883720930235E-2</v>
+      </c>
+      <c r="L17" s="42">
+        <f t="shared" si="5"/>
+        <v>0.50736395348837215</v>
+      </c>
+      <c r="M17" s="42">
+        <f t="shared" si="6"/>
+        <v>0.1666651162790698</v>
+      </c>
+      <c r="N17" s="48">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <v>1</v>
+      </c>
+      <c r="B18" s="47">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="47">
+        <f>C$16-($A18-$A$16)*C$10</f>
+        <v>2.2566899999999999</v>
+      </c>
+      <c r="D18" s="47">
+        <f>D$16-($A18-$A$16)*D$10</f>
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="E18" s="47">
+        <f>E$16-($A18-$A$16)*E$10</f>
+        <v>4.1433100000000005</v>
+      </c>
+      <c r="F18" s="47">
+        <f>F$16-($A18-$A$16)*F$10</f>
+        <v>1.3333000000000002</v>
+      </c>
+      <c r="G18" s="47">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I18" s="47">
+        <f>B18</f>
+        <v>8</v>
+      </c>
+      <c r="J18" s="42">
+        <f t="shared" si="3"/>
+        <v>0.28208624999999998</v>
+      </c>
+      <c r="K18" s="42">
+        <f t="shared" si="4"/>
+        <v>3.3337499999999999E-2</v>
+      </c>
+      <c r="L18" s="42">
+        <f t="shared" si="5"/>
+        <v>0.51791375000000006</v>
+      </c>
+      <c r="M18" s="42">
+        <f t="shared" si="6"/>
+        <v>0.16666250000000002</v>
+      </c>
+      <c r="N18" s="48">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="B19" s="47">
+        <f t="shared" si="8"/>
+        <v>7.5</v>
+      </c>
+      <c r="C19" s="47">
+        <f>C$16-($A19-$A$16)*C$10</f>
+        <v>2.0400399999999994</v>
+      </c>
+      <c r="D19" s="47">
+        <f>D$16-($A19-$A$16)*D$10</f>
+        <v>0.25004999999999999</v>
+      </c>
+      <c r="E19" s="47">
+        <f>E$16-($A19-$A$16)*E$10</f>
+        <v>3.9599600000000001</v>
+      </c>
+      <c r="F19" s="47">
+        <f>F$16-($A19-$A$16)*F$10</f>
+        <v>1.2499500000000001</v>
+      </c>
+      <c r="G19" s="47">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="I19" s="47">
+        <f>B19</f>
+        <v>7.5</v>
+      </c>
+      <c r="J19" s="42">
+        <f t="shared" si="3"/>
+        <v>0.27200533333333327</v>
+      </c>
+      <c r="K19" s="42">
+        <f t="shared" si="4"/>
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="L19" s="42">
+        <f t="shared" si="5"/>
+        <v>0.52799466666666672</v>
+      </c>
+      <c r="M19" s="42">
+        <f t="shared" si="6"/>
+        <v>0.16666</v>
+      </c>
+      <c r="N19" s="48">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="B20" s="47">
+        <f t="shared" si="8"/>
+        <v>6.3</v>
+      </c>
+      <c r="C20" s="47">
+        <f>C$19-($A20-$A$19)*C$10</f>
+        <v>1.5200799999999992</v>
+      </c>
+      <c r="D20" s="47">
+        <f>D$19-($A20-$A$19)*D$10</f>
+        <v>0.21009</v>
+      </c>
+      <c r="E20" s="47">
+        <f>E$19-($A20-$A$19)*E$10</f>
+        <v>3.5199199999999999</v>
+      </c>
+      <c r="F20" s="47">
+        <f>F$19-($A20-$A$19)*F$10</f>
+        <v>1.0499100000000001</v>
+      </c>
+      <c r="G20" s="47">
+        <f t="shared" si="2"/>
+        <v>6.2999999999999989</v>
+      </c>
+      <c r="I20" s="47">
+        <f>B20</f>
+        <v>6.3</v>
+      </c>
+      <c r="J20" s="42">
+        <f t="shared" si="3"/>
+        <v>0.24128253968253957</v>
+      </c>
+      <c r="K20" s="42">
+        <f t="shared" si="4"/>
+        <v>3.334761904761905E-2</v>
+      </c>
+      <c r="L20" s="42">
+        <f t="shared" si="5"/>
+        <v>0.55871746031746028</v>
+      </c>
+      <c r="M20" s="42">
+        <f t="shared" si="6"/>
+        <v>0.16665238095238097</v>
+      </c>
+      <c r="N20" s="48">
+        <f t="shared" si="7"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>

</xml_diff>

<commit_message>
Finish appendix and table of share of available water
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D196E4-33A5-4D82-AC6A-998572A19A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC03D359-8C92-4962-8E61-C4ACA7748173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="146">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -430,19 +430,82 @@
     <t>To be determined</t>
   </si>
   <si>
-    <t>Avaliable Water (maf per year) [2]</t>
-  </si>
-  <si>
-    <t>Total Shortage (maf per year) [1]</t>
-  </si>
-  <si>
     <t>Lower Basin Water Shortages</t>
   </si>
   <si>
     <t>Total Shortage (maf per year)</t>
   </si>
   <si>
-    <t>0 (Historical Allocation)</t>
+    <t>Share of Available Water (maf per year)</t>
+  </si>
+  <si>
+    <t>Percentage of Available Water</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>Total Shortage (maf per year) [A]</t>
+  </si>
+  <si>
+    <t>Avaliable Water (maf per year) [B]</t>
+  </si>
+  <si>
+    <t>Arizona [C]</t>
+  </si>
+  <si>
+    <t>Nevada [D]</t>
+  </si>
+  <si>
+    <t>California [E]</t>
+  </si>
+  <si>
+    <t>Mexico [F]</t>
+  </si>
+  <si>
+    <t>Total [G]</t>
+  </si>
+  <si>
+    <t>Arizona [H]</t>
+  </si>
+  <si>
+    <t>Nevada [I]</t>
+  </si>
+  <si>
+    <t>California [J]</t>
+  </si>
+  <si>
+    <t>Mexico [K]</t>
+  </si>
+  <si>
+    <t>Total [L]</t>
+  </si>
+  <si>
+    <t>[7]*</t>
+  </si>
+  <si>
+    <t>Percentage of Total Shortage</t>
+  </si>
+  <si>
+    <t>* If percentage shares of total shortages for 0.3 to 1.5 maf per year are propegated to total shortages for 1.5 to 2.7 maf per year.</t>
   </si>
 </sst>
 </file>
@@ -455,7 +518,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -494,7 +557,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,8 +576,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -572,13 +647,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -669,36 +766,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1132,488 +1261,556 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460CD49-F28E-4E8F-9EC7-325148866036}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="7.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="44" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="45" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+    </row>
+    <row r="7" spans="1:13" s="40" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="43"/>
+      <c r="D7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="E7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="F7" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="G7" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="H7" s="35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
-        <v>0</v>
-      </c>
-      <c r="C8" s="42">
-        <v>0</v>
-      </c>
-      <c r="D8" s="42">
-        <v>0</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0</v>
-      </c>
-      <c r="F8" s="42">
-        <v>0</v>
-      </c>
-      <c r="G8" s="42">
-        <f>SUM(C8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C8" s="39">
+        <v>0</v>
+      </c>
+      <c r="D8" s="48">
+        <v>0</v>
+      </c>
+      <c r="E8" s="48">
+        <v>0</v>
+      </c>
+      <c r="F8" s="48">
+        <v>0</v>
+      </c>
+      <c r="G8" s="48">
+        <v>0</v>
+      </c>
+      <c r="H8" s="48">
+        <f>SUM(D8:G8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="43">
+      <c r="D9" s="49">
         <v>0.8</v>
       </c>
-      <c r="D9" s="43">
+      <c r="E9" s="49">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E9" s="43">
-        <v>0</v>
-      </c>
-      <c r="F9" s="43">
+      <c r="F9" s="49">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G9" s="43">
-        <f t="shared" ref="G9:G10" si="0">SUM(C9:F9)</f>
+      <c r="H9" s="49">
+        <f t="shared" ref="H9:H10" si="0">SUM(D9:G9)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="43">
+      <c r="D10" s="49">
         <v>0.43330000000000002</v>
       </c>
-      <c r="D10" s="43">
+      <c r="E10" s="49">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E10" s="43">
+      <c r="F10" s="49">
         <v>0.36670000000000003</v>
       </c>
-      <c r="F10" s="43">
+      <c r="G10" s="49">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G10" s="43">
+      <c r="H10" s="49">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C11" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="D11" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="41"/>
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
       <c r="G11" s="41"/>
-    </row>
-    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="46" t="str">
-        <f>B14</f>
-        <v>Avaliable Water (maf per year) [2]</v>
-      </c>
-      <c r="J14" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="L14" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="49" t="s">
+      <c r="H11" s="41"/>
+    </row>
+    <row r="13" spans="1:13" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="50">
-        <f>G15-0</f>
+      <c r="B13" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="K14" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="L14" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14" s="55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="45">
+        <v>0</v>
+      </c>
+      <c r="C15" s="46">
+        <f>H15-0</f>
         <v>9</v>
       </c>
-      <c r="C15" s="50">
+      <c r="D15" s="31">
         <v>2.8</v>
       </c>
-      <c r="D15" s="50">
+      <c r="E15" s="31">
         <v>0.3</v>
       </c>
-      <c r="E15" s="50">
+      <c r="F15" s="31">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F15" s="50">
+      <c r="G15" s="31">
         <v>1.5</v>
       </c>
-      <c r="G15" s="50">
-        <f>SUM(C15:F15)</f>
+      <c r="H15" s="31">
+        <f>SUM(D15:G15)</f>
         <v>9</v>
       </c>
-      <c r="I15" s="47">
-        <f>B15</f>
-        <v>9</v>
-      </c>
-      <c r="J15" s="42">
-        <f>C15/$B15</f>
+      <c r="I15" s="50">
+        <f>D15/$C15</f>
         <v>0.31111111111111112</v>
       </c>
-      <c r="K15" s="42">
-        <f t="shared" ref="K15:M15" si="1">D15/$B15</f>
+      <c r="J15" s="50">
+        <f>E15/$C15</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="L15" s="42">
+      <c r="K15" s="50">
+        <f>F15/$C15</f>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="L15" s="50">
+        <f>G15/$C15</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M15" s="51">
+        <f>SUM(I15:L15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="47">
+        <f>C$15-B16</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D16" s="60">
+        <f>D15-$B16*D9</f>
+        <v>2.5599999999999996</v>
+      </c>
+      <c r="E16" s="60">
+        <f>E15-$B16*E9</f>
+        <v>0.29000999999999999</v>
+      </c>
+      <c r="F16" s="60">
+        <f>F15-$B16*F9</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G16" s="60">
+        <f>G15-$B16*G9</f>
+        <v>1.4499900000000001</v>
+      </c>
+      <c r="H16" s="60">
+        <f t="shared" ref="H16:H21" si="1">SUM(D16:G16)</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I16" s="50">
+        <f>D16/$C16</f>
+        <v>0.29425287356321839</v>
+      </c>
+      <c r="J16" s="50">
+        <f>E16/$C16</f>
+        <v>3.3334482758620693E-2</v>
+      </c>
+      <c r="K16" s="50">
+        <f>F16/$C16</f>
+        <v>0.50574712643678166</v>
+      </c>
+      <c r="L16" s="50">
+        <f>G16/$C16</f>
+        <v>0.16666551724137935</v>
+      </c>
+      <c r="M16" s="51">
+        <f t="shared" ref="M16:M21" si="2">SUM(I16:L16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="C17" s="47">
+        <f t="shared" ref="C17:C21" si="3">C$15-B17</f>
+        <v>8.6</v>
+      </c>
+      <c r="D17" s="60">
+        <f t="shared" ref="D17:G19" si="4">D$16-($B17-$B$16)*D$10</f>
+        <v>2.5166699999999995</v>
+      </c>
+      <c r="E17" s="60">
+        <f t="shared" si="4"/>
+        <v>0.28667999999999999</v>
+      </c>
+      <c r="F17" s="60">
+        <f t="shared" si="4"/>
+        <v>4.3633300000000004</v>
+      </c>
+      <c r="G17" s="60">
+        <f t="shared" si="4"/>
+        <v>1.4333200000000001</v>
+      </c>
+      <c r="H17" s="60">
         <f t="shared" si="1"/>
-        <v>0.48888888888888893</v>
-      </c>
-      <c r="M15" s="42">
+        <v>8.6</v>
+      </c>
+      <c r="I17" s="50">
+        <f>D17/$C17</f>
+        <v>0.29263604651162789</v>
+      </c>
+      <c r="J17" s="50">
+        <f>E17/$C17</f>
+        <v>3.3334883720930235E-2</v>
+      </c>
+      <c r="K17" s="50">
+        <f>F17/$C17</f>
+        <v>0.50736395348837215</v>
+      </c>
+      <c r="L17" s="50">
+        <f>G17/$C17</f>
+        <v>0.1666651162790698</v>
+      </c>
+      <c r="M17" s="51">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="39">
+        <v>1</v>
+      </c>
+      <c r="C18" s="47">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="D18" s="60">
+        <f t="shared" si="4"/>
+        <v>2.2566899999999999</v>
+      </c>
+      <c r="E18" s="60">
+        <f t="shared" si="4"/>
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="F18" s="60">
+        <f t="shared" si="4"/>
+        <v>4.1433100000000005</v>
+      </c>
+      <c r="G18" s="60">
+        <f t="shared" si="4"/>
+        <v>1.3333000000000002</v>
+      </c>
+      <c r="H18" s="60">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="N15" s="48">
-        <f>SUM(J15:M15)</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="50">
+        <f>D18/$C18</f>
+        <v>0.28208624999999998</v>
+      </c>
+      <c r="J18" s="50">
+        <f>E18/$C18</f>
+        <v>3.3337499999999999E-2</v>
+      </c>
+      <c r="K18" s="50">
+        <f>F18/$C18</f>
+        <v>0.51791375000000006</v>
+      </c>
+      <c r="L18" s="50">
+        <f>G18/$C18</f>
+        <v>0.16666250000000002</v>
+      </c>
+      <c r="M18" s="51">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="B16" s="47">
-        <f>B$15-A16</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C16" s="47">
-        <f>C15-$A16*C9</f>
-        <v>2.5599999999999996</v>
-      </c>
-      <c r="D16" s="47">
-        <f>D15-$A16*D9</f>
-        <v>0.29000999999999999</v>
-      </c>
-      <c r="E16" s="47">
-        <f>E15-$A16*E9</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F16" s="47">
-        <f>F15-$A16*F9</f>
-        <v>1.4499900000000001</v>
-      </c>
-      <c r="G16" s="47">
-        <f t="shared" ref="G16:G20" si="2">SUM(C16:F16)</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="I16" s="47">
-        <f>B16</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="J16" s="42">
-        <f t="shared" ref="J16:J20" si="3">C16/$B16</f>
-        <v>0.29425287356321839</v>
-      </c>
-      <c r="K16" s="42">
-        <f t="shared" ref="K16:K20" si="4">D16/$B16</f>
-        <v>3.3334482758620693E-2</v>
-      </c>
-      <c r="L16" s="42">
-        <f t="shared" ref="L16:L20" si="5">E16/$B16</f>
-        <v>0.50574712643678166</v>
-      </c>
-      <c r="M16" s="42">
-        <f t="shared" ref="M16:M20" si="6">F16/$B16</f>
-        <v>0.16666551724137935</v>
-      </c>
-      <c r="N16" s="48">
-        <f t="shared" ref="N16:N20" si="7">SUM(J16:M16)</f>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="47">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="D19" s="60">
+        <f t="shared" si="4"/>
+        <v>2.0400399999999994</v>
+      </c>
+      <c r="E19" s="60">
+        <f t="shared" si="4"/>
+        <v>0.25004999999999999</v>
+      </c>
+      <c r="F19" s="60">
+        <f t="shared" si="4"/>
+        <v>3.9599600000000001</v>
+      </c>
+      <c r="G19" s="60">
+        <f t="shared" si="4"/>
+        <v>1.2499500000000001</v>
+      </c>
+      <c r="H19" s="60">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="I19" s="50">
+        <f>D19/$C19</f>
+        <v>0.27200533333333327</v>
+      </c>
+      <c r="J19" s="50">
+        <f>E19/$C19</f>
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="K19" s="50">
+        <f>F19/$C19</f>
+        <v>0.52799466666666672</v>
+      </c>
+      <c r="L19" s="50">
+        <f>G19/$C19</f>
+        <v>0.16666</v>
+      </c>
+      <c r="M19" s="51">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="B17" s="47">
-        <f t="shared" ref="B17:B20" si="8">B$15-A17</f>
-        <v>8.6</v>
-      </c>
-      <c r="C17" s="47">
-        <f>C$16-($A17-$A$16)*C$10</f>
-        <v>2.5166699999999995</v>
-      </c>
-      <c r="D17" s="47">
-        <f>D$16-($A17-$A$16)*D$10</f>
-        <v>0.28667999999999999</v>
-      </c>
-      <c r="E17" s="47">
-        <f>E$16-($A17-$A$16)*E$10</f>
-        <v>4.3633300000000004</v>
-      </c>
-      <c r="F17" s="47">
-        <f>F$16-($A17-$A$16)*F$10</f>
-        <v>1.4333200000000001</v>
-      </c>
-      <c r="G17" s="47">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="39">
+        <v>2.7</v>
+      </c>
+      <c r="C20" s="47">
+        <f t="shared" si="3"/>
+        <v>6.3</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="58"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="39">
+        <v>2.7</v>
+      </c>
+      <c r="C21" s="47">
+        <f t="shared" si="3"/>
+        <v>6.3</v>
+      </c>
+      <c r="D21" s="60">
+        <f>D$19-($B21-$B$19)*D$10</f>
+        <v>1.5200799999999992</v>
+      </c>
+      <c r="E21" s="60">
+        <f>E$19-($B21-$B$19)*E$10</f>
+        <v>0.21009</v>
+      </c>
+      <c r="F21" s="60">
+        <f>F$19-($B21-$B$19)*F$10</f>
+        <v>3.5199199999999999</v>
+      </c>
+      <c r="G21" s="60">
+        <f>G$19-($B21-$B$19)*G$10</f>
+        <v>1.0499100000000001</v>
+      </c>
+      <c r="H21" s="60">
+        <f t="shared" si="1"/>
+        <v>6.2999999999999989</v>
+      </c>
+      <c r="I21" s="50">
+        <f>D21/$C21</f>
+        <v>0.24128253968253957</v>
+      </c>
+      <c r="J21" s="50">
+        <f>E21/$C21</f>
+        <v>3.334761904761905E-2</v>
+      </c>
+      <c r="K21" s="50">
+        <f>F21/$C21</f>
+        <v>0.55871746031746028</v>
+      </c>
+      <c r="L21" s="50">
+        <f>G21/$C21</f>
+        <v>0.16665238095238097</v>
+      </c>
+      <c r="M21" s="51">
         <f t="shared" si="2"/>
-        <v>8.6</v>
-      </c>
-      <c r="I17" s="47">
-        <f>B17</f>
-        <v>8.6</v>
-      </c>
-      <c r="J17" s="42">
-        <f t="shared" si="3"/>
-        <v>0.29263604651162789</v>
-      </c>
-      <c r="K17" s="42">
-        <f t="shared" si="4"/>
-        <v>3.3334883720930235E-2</v>
-      </c>
-      <c r="L17" s="42">
-        <f t="shared" si="5"/>
-        <v>0.50736395348837215</v>
-      </c>
-      <c r="M17" s="42">
-        <f t="shared" si="6"/>
-        <v>0.1666651162790698</v>
-      </c>
-      <c r="N17" s="48">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="12">
-        <v>1</v>
-      </c>
-      <c r="B18" s="47">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="C18" s="47">
-        <f>C$16-($A18-$A$16)*C$10</f>
-        <v>2.2566899999999999</v>
-      </c>
-      <c r="D18" s="47">
-        <f>D$16-($A18-$A$16)*D$10</f>
-        <v>0.26669999999999999</v>
-      </c>
-      <c r="E18" s="47">
-        <f>E$16-($A18-$A$16)*E$10</f>
-        <v>4.1433100000000005</v>
-      </c>
-      <c r="F18" s="47">
-        <f>F$16-($A18-$A$16)*F$10</f>
-        <v>1.3333000000000002</v>
-      </c>
-      <c r="G18" s="47">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="I18" s="47">
-        <f>B18</f>
-        <v>8</v>
-      </c>
-      <c r="J18" s="42">
-        <f t="shared" si="3"/>
-        <v>0.28208624999999998</v>
-      </c>
-      <c r="K18" s="42">
-        <f t="shared" si="4"/>
-        <v>3.3337499999999999E-2</v>
-      </c>
-      <c r="L18" s="42">
-        <f t="shared" si="5"/>
-        <v>0.51791375000000006</v>
-      </c>
-      <c r="M18" s="42">
-        <f t="shared" si="6"/>
-        <v>0.16666250000000002</v>
-      </c>
-      <c r="N18" s="48">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="B19" s="47">
-        <f t="shared" si="8"/>
-        <v>7.5</v>
-      </c>
-      <c r="C19" s="47">
-        <f>C$16-($A19-$A$16)*C$10</f>
-        <v>2.0400399999999994</v>
-      </c>
-      <c r="D19" s="47">
-        <f>D$16-($A19-$A$16)*D$10</f>
-        <v>0.25004999999999999</v>
-      </c>
-      <c r="E19" s="47">
-        <f>E$16-($A19-$A$16)*E$10</f>
-        <v>3.9599600000000001</v>
-      </c>
-      <c r="F19" s="47">
-        <f>F$16-($A19-$A$16)*F$10</f>
-        <v>1.2499500000000001</v>
-      </c>
-      <c r="G19" s="47">
-        <f t="shared" si="2"/>
-        <v>7.5</v>
-      </c>
-      <c r="I19" s="47">
-        <f>B19</f>
-        <v>7.5</v>
-      </c>
-      <c r="J19" s="42">
-        <f t="shared" si="3"/>
-        <v>0.27200533333333327</v>
-      </c>
-      <c r="K19" s="42">
-        <f t="shared" si="4"/>
-        <v>3.3340000000000002E-2</v>
-      </c>
-      <c r="L19" s="42">
-        <f t="shared" si="5"/>
-        <v>0.52799466666666672</v>
-      </c>
-      <c r="M19" s="42">
-        <f t="shared" si="6"/>
-        <v>0.16666</v>
-      </c>
-      <c r="N19" s="48">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="12">
-        <v>2.7</v>
-      </c>
-      <c r="B20" s="47">
-        <f t="shared" si="8"/>
-        <v>6.3</v>
-      </c>
-      <c r="C20" s="47">
-        <f>C$19-($A20-$A$19)*C$10</f>
-        <v>1.5200799999999992</v>
-      </c>
-      <c r="D20" s="47">
-        <f>D$19-($A20-$A$19)*D$10</f>
-        <v>0.21009</v>
-      </c>
-      <c r="E20" s="47">
-        <f>E$19-($A20-$A$19)*E$10</f>
-        <v>3.5199199999999999</v>
-      </c>
-      <c r="F20" s="47">
-        <f>F$19-($A20-$A$19)*F$10</f>
-        <v>1.0499100000000001</v>
-      </c>
-      <c r="G20" s="47">
-        <f t="shared" si="2"/>
-        <v>6.2999999999999989</v>
-      </c>
-      <c r="I20" s="47">
-        <f>B20</f>
-        <v>6.3</v>
-      </c>
-      <c r="J20" s="42">
-        <f t="shared" si="3"/>
-        <v>0.24128253968253957</v>
-      </c>
-      <c r="K20" s="42">
-        <f t="shared" si="4"/>
-        <v>3.334761904761905E-2</v>
-      </c>
-      <c r="L20" s="42">
-        <f t="shared" si="5"/>
-        <v>0.55871746031746028</v>
-      </c>
-      <c r="M20" s="42">
-        <f t="shared" si="6"/>
-        <v>0.16665238095238097</v>
-      </c>
-      <c r="N20" s="48">
-        <f t="shared" si="7"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="59" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C11:G11"/>
+  <mergeCells count="10">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="I13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3803,14 +4000,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -3906,10 +4103,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>
@@ -4014,10 +4211,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Final versions of word doc and excel sheet
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC03D359-8C92-4962-8E61-C4ACA7748173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFD70E3-0229-4E4E-9187-5F29F3CED6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1995" windowWidth="20640" windowHeight="11040" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="148">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -430,9 +430,6 @@
     <t>To be determined</t>
   </si>
   <si>
-    <t>Lower Basin Water Shortages</t>
-  </si>
-  <si>
     <t>Total Shortage (maf per year)</t>
   </si>
   <si>
@@ -445,9 +442,6 @@
     <t>Row</t>
   </si>
   <si>
-    <t>[1]</t>
-  </si>
-  <si>
     <t>[2]</t>
   </si>
   <si>
@@ -499,13 +493,25 @@
     <t>Total [L]</t>
   </si>
   <si>
-    <t>[7]*</t>
-  </si>
-  <si>
-    <t>Percentage of Total Shortage</t>
-  </si>
-  <si>
-    <t>* If percentage shares of total shortages for 0.3 to 1.5 maf per year are propegated to total shortages for 1.5 to 2.7 maf per year.</t>
+    <t>As Volume (maf per year)</t>
+  </si>
+  <si>
+    <t>[1]*</t>
+  </si>
+  <si>
+    <t>[7]**</t>
+  </si>
+  <si>
+    <t>** If percentage shares of total shortages for 0.3 to 1.5 maf per year are propegated to total shortages for 1.5 to 2.7 maf per year.</t>
+  </si>
+  <si>
+    <t>* Historical allocations</t>
+  </si>
+  <si>
+    <t>7.5 to 6.3</t>
+  </si>
+  <si>
+    <t>As Percent of Total Shortage</t>
   </si>
 </sst>
 </file>
@@ -520,7 +526,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +558,25 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -589,7 +614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -662,11 +687,46 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -675,7 +735,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -766,68 +826,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1261,72 +1370,183 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460CD49-F28E-4E8F-9EC7-325148866036}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
-    <col min="5" max="5" width="7.90625" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" customWidth="1"/>
+    <col min="1" max="1" width="5.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="5.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.08984375" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="7.08984375" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" customWidth="1"/>
+    <col min="16" max="16" width="6.81640625" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+    <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="73"/>
+    </row>
+    <row r="6" spans="1:21" s="41" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-    </row>
-    <row r="7" spans="1:13" s="40" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="43"/>
-      <c r="D7" s="35" t="s">
+      <c r="C6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="D6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="E6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="F6" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="G6" s="42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C8" s="39">
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="M6" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="N6" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="O6" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="P6" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q6" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="R6" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="S6" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="T6" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="U6" s="56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="41" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
+      <c r="I7" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" s="57">
+        <f>B13</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="58">
+        <v>9</v>
+      </c>
+      <c r="L7" s="59">
+        <v>2.8</v>
+      </c>
+      <c r="M7" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="N7" s="59">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O7" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="P7" s="59">
+        <f>SUM(L7:O7)</f>
+        <v>9</v>
+      </c>
+      <c r="Q7" s="60">
+        <f>L7/$K7</f>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="R7" s="60">
+        <f>M7/$K7</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="S7" s="60">
+        <f>N7/$K7</f>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="T7" s="60">
+        <f>O7/$K7</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="U7" s="74">
+        <f>SUM(Q7:T7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B8" s="47">
+        <v>0</v>
+      </c>
+      <c r="C8" s="48">
         <v>0</v>
       </c>
       <c r="D8" s="48">
@@ -1339,478 +1559,562 @@
         <v>0</v>
       </c>
       <c r="G8" s="48">
-        <v>0</v>
-      </c>
-      <c r="H8" s="48">
-        <f>SUM(D8:G8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C9" s="39" t="s">
+        <f>SUM(C8:F8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="57">
+        <f>B14</f>
+        <v>0.3</v>
+      </c>
+      <c r="K8" s="61">
+        <f>K$7-J8</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L8" s="54">
+        <f>L$7-C14</f>
+        <v>2.5599999999999996</v>
+      </c>
+      <c r="M8" s="54">
+        <f>M$7-D14</f>
+        <v>0.29000999999999999</v>
+      </c>
+      <c r="N8" s="54">
+        <f>N$7-E14</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O8" s="54">
+        <f>O$7-F14</f>
+        <v>1.4499900000000001</v>
+      </c>
+      <c r="P8" s="59">
+        <f t="shared" ref="P8:P11" si="0">SUM(L8:O8)</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="Q8" s="60">
+        <f>L8/$K8</f>
+        <v>0.29425287356321839</v>
+      </c>
+      <c r="R8" s="60">
+        <f>M8/$K8</f>
+        <v>3.3334482758620693E-2</v>
+      </c>
+      <c r="S8" s="60">
+        <f>N8/$K8</f>
+        <v>0.50574712643678166</v>
+      </c>
+      <c r="T8" s="60">
+        <f>O8/$K8</f>
+        <v>0.16666551724137935</v>
+      </c>
+      <c r="U8" s="74">
+        <f t="shared" ref="U8:U13" si="1">SUM(Q8:T8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B9" s="47" t="s">
         <v>116</v>
       </c>
+      <c r="C9" s="49">
+        <v>0.8</v>
+      </c>
       <c r="D9" s="49">
-        <v>0.8</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="E9" s="49">
+        <v>0</v>
+      </c>
+      <c r="F9" s="49">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G9" s="49">
+        <f t="shared" ref="G9:G10" si="2">SUM(C9:F9)</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="57">
+        <f>B15</f>
+        <v>0.4</v>
+      </c>
+      <c r="K9" s="61">
+        <f>K$7-J9</f>
+        <v>8.6</v>
+      </c>
+      <c r="L9" s="54">
+        <f>L$7-C15</f>
+        <v>2.51667</v>
+      </c>
+      <c r="M9" s="54">
+        <f>M$7-D15</f>
+        <v>0.28667999999999999</v>
+      </c>
+      <c r="N9" s="54">
+        <f>N$7-E15</f>
+        <v>4.3633300000000004</v>
+      </c>
+      <c r="O9" s="54">
+        <f>O$7-F15</f>
+        <v>1.4333199999999999</v>
+      </c>
+      <c r="P9" s="59">
+        <f t="shared" si="0"/>
+        <v>8.6</v>
+      </c>
+      <c r="Q9" s="60">
+        <f>L9/$K9</f>
+        <v>0.29263604651162789</v>
+      </c>
+      <c r="R9" s="60">
+        <f>M9/$K9</f>
+        <v>3.3334883720930235E-2</v>
+      </c>
+      <c r="S9" s="60">
+        <f>N9/$K9</f>
+        <v>0.50736395348837215</v>
+      </c>
+      <c r="T9" s="60">
+        <f>O9/$K9</f>
+        <v>0.16666511627906977</v>
+      </c>
+      <c r="U9" s="74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B10" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="49">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="D10" s="49">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="F9" s="49">
-        <v>0</v>
-      </c>
-      <c r="G9" s="49">
+      <c r="E10" s="49">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="F10" s="49">
         <v>0.16669999999999999</v>
       </c>
-      <c r="H9" s="49">
-        <f t="shared" ref="H9:H10" si="0">SUM(D9:G9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C10" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="49">
-        <v>0.43330000000000002</v>
-      </c>
-      <c r="E10" s="49">
-        <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="F10" s="49">
-        <v>0.36670000000000003</v>
-      </c>
       <c r="G10" s="49">
-        <v>0.16669999999999999</v>
-      </c>
-      <c r="H10" s="49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C11" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-    </row>
-    <row r="13" spans="1:13" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-    </row>
-    <row r="14" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="J14" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="K14" s="55" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" s="55" t="s">
-        <v>141</v>
-      </c>
-      <c r="M14" s="55" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="45">
-        <v>0</v>
-      </c>
-      <c r="C15" s="46">
-        <f>H15-0</f>
-        <v>9</v>
-      </c>
-      <c r="D15" s="31">
-        <v>2.8</v>
-      </c>
-      <c r="E15" s="31">
-        <v>0.3</v>
-      </c>
-      <c r="F15" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G15" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="H15" s="31">
-        <f>SUM(D15:G15)</f>
-        <v>9</v>
-      </c>
-      <c r="I15" s="50">
-        <f>D15/$C15</f>
-        <v>0.31111111111111112</v>
-      </c>
-      <c r="J15" s="50">
-        <f>E15/$C15</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="K15" s="50">
-        <f>F15/$C15</f>
-        <v>0.48888888888888893</v>
-      </c>
-      <c r="L15" s="50">
-        <f>G15/$C15</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M15" s="51">
-        <f>SUM(I15:L15)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="39">
-        <v>0.3</v>
-      </c>
-      <c r="C16" s="47">
-        <f>C$15-B16</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D16" s="60">
-        <f>D15-$B16*D9</f>
-        <v>2.5599999999999996</v>
-      </c>
-      <c r="E16" s="60">
-        <f>E15-$B16*E9</f>
-        <v>0.29000999999999999</v>
-      </c>
-      <c r="F16" s="60">
-        <f>F15-$B16*F9</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G16" s="60">
-        <f>G15-$B16*G9</f>
-        <v>1.4499900000000001</v>
-      </c>
-      <c r="H16" s="60">
-        <f t="shared" ref="H16:H21" si="1">SUM(D16:G16)</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="I16" s="50">
-        <f>D16/$C16</f>
-        <v>0.29425287356321839</v>
-      </c>
-      <c r="J16" s="50">
-        <f>E16/$C16</f>
-        <v>3.3334482758620693E-2</v>
-      </c>
-      <c r="K16" s="50">
-        <f>F16/$C16</f>
-        <v>0.50574712643678166</v>
-      </c>
-      <c r="L16" s="50">
-        <f>G16/$C16</f>
-        <v>0.16666551724137935</v>
-      </c>
-      <c r="M16" s="51">
-        <f t="shared" ref="M16:M21" si="2">SUM(I16:L16)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="39">
-        <v>0.4</v>
-      </c>
-      <c r="C17" s="47">
-        <f t="shared" ref="C17:C21" si="3">C$15-B17</f>
-        <v>8.6</v>
-      </c>
-      <c r="D17" s="60">
-        <f t="shared" ref="D17:G19" si="4">D$16-($B17-$B$16)*D$10</f>
-        <v>2.5166699999999995</v>
-      </c>
-      <c r="E17" s="60">
-        <f t="shared" si="4"/>
-        <v>0.28667999999999999</v>
-      </c>
-      <c r="F17" s="60">
-        <f t="shared" si="4"/>
-        <v>4.3633300000000004</v>
-      </c>
-      <c r="G17" s="60">
-        <f t="shared" si="4"/>
-        <v>1.4333200000000001</v>
-      </c>
-      <c r="H17" s="60">
-        <f t="shared" si="1"/>
-        <v>8.6</v>
-      </c>
-      <c r="I17" s="50">
-        <f>D17/$C17</f>
-        <v>0.29263604651162789</v>
-      </c>
-      <c r="J17" s="50">
-        <f>E17/$C17</f>
-        <v>3.3334883720930235E-2</v>
-      </c>
-      <c r="K17" s="50">
-        <f>F17/$C17</f>
-        <v>0.50736395348837215</v>
-      </c>
-      <c r="L17" s="50">
-        <f>G17/$C17</f>
-        <v>0.1666651162790698</v>
-      </c>
-      <c r="M17" s="51">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="32" t="s">
+      <c r="I10" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="57">
+        <f>B16</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="61">
+        <f>K$7-J10</f>
+        <v>8</v>
+      </c>
+      <c r="L10" s="54">
+        <f>L$7-C16</f>
+        <v>2.2566899999999999</v>
+      </c>
+      <c r="M10" s="54">
+        <f>M$7-D16</f>
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="N10" s="54">
+        <f>N$7-E16</f>
+        <v>4.1433100000000005</v>
+      </c>
+      <c r="O10" s="54">
+        <f>O$7-F16</f>
+        <v>1.3332999999999999</v>
+      </c>
+      <c r="P10" s="59">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Q10" s="60">
+        <f>L10/$K10</f>
+        <v>0.28208624999999998</v>
+      </c>
+      <c r="R10" s="60">
+        <f>M10/$K10</f>
+        <v>3.3337499999999999E-2</v>
+      </c>
+      <c r="S10" s="60">
+        <f>N10/$K10</f>
+        <v>0.51791375000000006</v>
+      </c>
+      <c r="T10" s="60">
+        <f>O10/$K10</f>
+        <v>0.16666249999999999</v>
+      </c>
+      <c r="U10" s="74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B11" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="I11" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="57">
+        <f>B17</f>
+        <v>1.5</v>
+      </c>
+      <c r="K11" s="61">
+        <f>K$7-J11</f>
+        <v>7.5</v>
+      </c>
+      <c r="L11" s="54">
+        <f>L$7-C17</f>
+        <v>2.0400399999999999</v>
+      </c>
+      <c r="M11" s="54">
+        <f>M$7-D17</f>
+        <v>0.25004999999999999</v>
+      </c>
+      <c r="N11" s="54">
+        <f>N$7-E17</f>
+        <v>3.9599600000000001</v>
+      </c>
+      <c r="O11" s="54">
+        <f>O$7-F17</f>
+        <v>1.2499500000000001</v>
+      </c>
+      <c r="P11" s="59">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="Q11" s="60">
+        <f>L11/$K11</f>
+        <v>0.27200533333333332</v>
+      </c>
+      <c r="R11" s="60">
+        <f>M11/$K11</f>
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="S11" s="60">
+        <f>N11/$K11</f>
+        <v>0.52799466666666672</v>
+      </c>
+      <c r="T11" s="60">
+        <f>O11/$K11</f>
+        <v>0.16666</v>
+      </c>
+      <c r="U11" s="74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B12" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="I12" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="39">
+      <c r="J12" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="L12" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="64"/>
+    </row>
+    <row r="13" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B13" s="47">
+        <v>0</v>
+      </c>
+      <c r="C13" s="53">
+        <v>0</v>
+      </c>
+      <c r="D13" s="53">
+        <v>0</v>
+      </c>
+      <c r="E13" s="53">
+        <v>0</v>
+      </c>
+      <c r="F13" s="53">
+        <v>0</v>
+      </c>
+      <c r="G13" s="53">
+        <f>SUM(C13:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="J13" s="57">
+        <v>2.7</v>
+      </c>
+      <c r="K13" s="61">
+        <f>K$7-J13</f>
+        <v>6.3</v>
+      </c>
+      <c r="L13" s="54">
+        <f>L11-C10*($K11-$K13)</f>
+        <v>1.5200799999999997</v>
+      </c>
+      <c r="M13" s="54">
+        <f>M11-D10*($K11-$K13)</f>
+        <v>0.21009</v>
+      </c>
+      <c r="N13" s="54">
+        <f>N11-E10*($K11-$K13)</f>
+        <v>3.5199199999999999</v>
+      </c>
+      <c r="O13" s="54">
+        <f>O11-F10*($K11-$K13)</f>
+        <v>1.0499100000000001</v>
+      </c>
+      <c r="P13" s="54">
+        <f>P11-G10*($K11-$K13)</f>
+        <v>6.3</v>
+      </c>
+      <c r="Q13" s="60">
+        <f>L13/$K13</f>
+        <v>0.24128253968253963</v>
+      </c>
+      <c r="R13" s="60">
+        <f>M13/$K13</f>
+        <v>3.334761904761905E-2</v>
+      </c>
+      <c r="S13" s="60">
+        <f>N13/$K13</f>
+        <v>0.55871746031746028</v>
+      </c>
+      <c r="T13" s="60">
+        <f>O13/$K13</f>
+        <v>0.16665238095238097</v>
+      </c>
+      <c r="U13" s="74">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C18" s="47">
+    </row>
+    <row r="14" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B14" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="54">
+        <f>$B14*C9</f>
+        <v>0.24</v>
+      </c>
+      <c r="D14" s="54">
+        <f>$B14*D9</f>
+        <v>9.9900000000000006E-3</v>
+      </c>
+      <c r="E14" s="54">
+        <f>$B14*E9</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="54">
+        <f>$B14*F9</f>
+        <v>5.0009999999999992E-2</v>
+      </c>
+      <c r="G14" s="54">
+        <f>SUM(C14:F14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="I14" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" s="68"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="67"/>
+      <c r="S14" s="67"/>
+      <c r="T14" s="67"/>
+      <c r="U14" s="75"/>
+    </row>
+    <row r="15" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B15" s="47">
+        <v>0.4</v>
+      </c>
+      <c r="C15" s="54">
+        <f>C$14+C$10*($B15-$B$14)</f>
+        <v>0.28333000000000003</v>
+      </c>
+      <c r="D15" s="54">
+        <f>D$14+D$10*($B15-$B$14)</f>
+        <v>1.3320000000000002E-2</v>
+      </c>
+      <c r="E15" s="54">
+        <f>E$14+E$10*($B15-$B$14)</f>
+        <v>3.6670000000000015E-2</v>
+      </c>
+      <c r="F15" s="54">
+        <f>F$14+F$10*($B15-$B$14)</f>
+        <v>6.6679999999999989E-2</v>
+      </c>
+      <c r="G15" s="54">
+        <f>SUM(C15:F15)</f>
+        <v>0.4</v>
+      </c>
+      <c r="I15" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="68"/>
+      <c r="U15" s="76"/>
+    </row>
+    <row r="16" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B16" s="47">
+        <v>1</v>
+      </c>
+      <c r="C16" s="54">
+        <f>C$14+C$10*($B16-$B$14)</f>
+        <v>0.54330999999999996</v>
+      </c>
+      <c r="D16" s="54">
+        <f>D$14+D$10*($B16-$B$14)</f>
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="E16" s="54">
+        <f>E$14+E$10*($B16-$B$14)</f>
+        <v>0.25669000000000003</v>
+      </c>
+      <c r="F16" s="54">
+        <f>F$14+F$10*($B16-$B$14)</f>
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G16" s="54">
+        <f t="shared" ref="G16:G17" si="3">SUM(C16:F16)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="U16" s="76"/>
+    </row>
+    <row r="17" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B17" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="54">
+        <f>C$14+C$10*($B17-$B$14)</f>
+        <v>0.75995999999999997</v>
+      </c>
+      <c r="D17" s="54">
+        <f>D$14+D$10*($B17-$B$14)</f>
+        <v>4.9950000000000001E-2</v>
+      </c>
+      <c r="E17" s="54">
+        <f>E$14+E$10*($B17-$B$14)</f>
+        <v>0.44004000000000004</v>
+      </c>
+      <c r="F17" s="54">
+        <f>F$14+F$10*($B17-$B$14)</f>
+        <v>0.25004999999999994</v>
+      </c>
+      <c r="G17" s="54">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="D18" s="60">
-        <f t="shared" si="4"/>
-        <v>2.2566899999999999</v>
-      </c>
-      <c r="E18" s="60">
-        <f t="shared" si="4"/>
-        <v>0.26669999999999999</v>
-      </c>
-      <c r="F18" s="60">
-        <f t="shared" si="4"/>
-        <v>4.1433100000000005</v>
-      </c>
-      <c r="G18" s="60">
-        <f t="shared" si="4"/>
-        <v>1.3333000000000002</v>
-      </c>
-      <c r="H18" s="60">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I18" s="50">
-        <f>D18/$C18</f>
-        <v>0.28208624999999998</v>
-      </c>
-      <c r="J18" s="50">
-        <f>E18/$C18</f>
-        <v>3.3337499999999999E-2</v>
-      </c>
-      <c r="K18" s="50">
-        <f>F18/$C18</f>
-        <v>0.51791375000000006</v>
-      </c>
-      <c r="L18" s="50">
-        <f>G18/$C18</f>
-        <v>0.16666250000000002</v>
-      </c>
-      <c r="M18" s="51">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="39">
         <v>1.5</v>
       </c>
-      <c r="C19" s="47">
-        <f t="shared" si="3"/>
-        <v>7.5</v>
-      </c>
-      <c r="D19" s="60">
-        <f t="shared" si="4"/>
-        <v>2.0400399999999994</v>
-      </c>
-      <c r="E19" s="60">
-        <f t="shared" si="4"/>
-        <v>0.25004999999999999</v>
-      </c>
-      <c r="F19" s="60">
-        <f t="shared" si="4"/>
-        <v>3.9599600000000001</v>
-      </c>
-      <c r="G19" s="60">
-        <f t="shared" si="4"/>
-        <v>1.2499500000000001</v>
-      </c>
-      <c r="H19" s="60">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="I19" s="50">
-        <f>D19/$C19</f>
-        <v>0.27200533333333327</v>
-      </c>
-      <c r="J19" s="50">
-        <f>E19/$C19</f>
-        <v>3.3340000000000002E-2</v>
-      </c>
-      <c r="K19" s="50">
-        <f>F19/$C19</f>
-        <v>0.52799466666666672</v>
-      </c>
-      <c r="L19" s="50">
-        <f>G19/$C19</f>
-        <v>0.16666</v>
-      </c>
-      <c r="M19" s="51">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="39">
-        <v>2.7</v>
-      </c>
-      <c r="C20" s="47">
-        <f t="shared" si="3"/>
-        <v>6.3</v>
-      </c>
-      <c r="D20" s="56" t="s">
+      <c r="U17" s="76"/>
+    </row>
+    <row r="18" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B18" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="58"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="39">
-        <v>2.7</v>
-      </c>
-      <c r="C21" s="47">
-        <f t="shared" si="3"/>
-        <v>6.3</v>
-      </c>
-      <c r="D21" s="60">
-        <f>D$19-($B21-$B$19)*D$10</f>
-        <v>1.5200799999999992</v>
-      </c>
-      <c r="E21" s="60">
-        <f>E$19-($B21-$B$19)*E$10</f>
-        <v>0.21009</v>
-      </c>
-      <c r="F21" s="60">
-        <f>F$19-($B21-$B$19)*F$10</f>
-        <v>3.5199199999999999</v>
-      </c>
-      <c r="G21" s="60">
-        <f>G$19-($B21-$B$19)*G$10</f>
-        <v>1.0499100000000001</v>
-      </c>
-      <c r="H21" s="60">
-        <f t="shared" si="1"/>
-        <v>6.2999999999999989</v>
-      </c>
-      <c r="I21" s="50">
-        <f>D21/$C21</f>
-        <v>0.24128253968253957</v>
-      </c>
-      <c r="J21" s="50">
-        <f>E21/$C21</f>
-        <v>3.334761904761905E-2</v>
-      </c>
-      <c r="K21" s="50">
-        <f>F21/$C21</f>
-        <v>0.55871746031746028</v>
-      </c>
-      <c r="L21" s="50">
-        <f>G21/$C21</f>
-        <v>0.16665238095238097</v>
-      </c>
-      <c r="M21" s="51">
-        <f t="shared" si="2"/>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="59" t="s">
-        <v>145</v>
-      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="U18" s="76"/>
+    </row>
+    <row r="19" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U19" s="76"/>
+    </row>
+    <row r="20" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U20" s="76"/>
+    </row>
+    <row r="21" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U21" s="76"/>
+    </row>
+    <row r="22" spans="2:21" s="46" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U22" s="76"/>
+    </row>
+    <row r="23" spans="2:21" s="46" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="76"/>
+    </row>
+    <row r="24" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U24" s="76"/>
+    </row>
+    <row r="25" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U25" s="76"/>
+    </row>
+    <row r="26" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U26" s="76"/>
+    </row>
+    <row r="27" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U27" s="76"/>
+    </row>
+    <row r="28" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U28" s="76"/>
+    </row>
+    <row r="29" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U29" s="76"/>
+    </row>
+    <row r="30" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U30" s="76"/>
+    </row>
+    <row r="31" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U31" s="76"/>
+    </row>
+    <row r="32" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U32" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="I13:M13"/>
+  <mergeCells count="11">
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="L12:P12"/>
+    <mergeCell ref="Q12:U12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4000,14 +4304,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -4103,10 +4407,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="42"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>
@@ -4211,10 +4515,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="42"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Update Lake Mead Water conservation program analysis as a suggested alternative post 2026
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFD70E3-0229-4E4E-9187-5F29F3CED6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380EEAA-90CF-45CF-97A5-F434335BACB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="20640" windowHeight="11040" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -433,12 +433,6 @@
     <t>Total Shortage (maf per year)</t>
   </si>
   <si>
-    <t>Share of Available Water (maf per year)</t>
-  </si>
-  <si>
-    <t>Percentage of Available Water</t>
-  </si>
-  <si>
     <t>Row</t>
   </si>
   <si>
@@ -460,9 +454,6 @@
     <t>Total Shortage (maf per year) [A]</t>
   </si>
   <si>
-    <t>Avaliable Water (maf per year) [B]</t>
-  </si>
-  <si>
     <t>Arizona [C]</t>
   </si>
   <si>
@@ -502,9 +493,6 @@
     <t>[7]**</t>
   </si>
   <si>
-    <t>** If percentage shares of total shortages for 0.3 to 1.5 maf per year are propegated to total shortages for 1.5 to 2.7 maf per year.</t>
-  </si>
-  <si>
     <t>* Historical allocations</t>
   </si>
   <si>
@@ -512,6 +500,18 @@
   </si>
   <si>
     <t>As Percent of Total Shortage</t>
+  </si>
+  <si>
+    <t>Share of Lake Mead Inflow (maf per year)</t>
+  </si>
+  <si>
+    <t>Lake Mead Inflow (maf per year) [B]</t>
+  </si>
+  <si>
+    <t>Percentage of Lake Mead Inflow</t>
+  </si>
+  <si>
+    <t>** If percentage shares of total shortages for 0.3 to 1.5 maf per year are continue to total shortages for 1.5 to 2.7 maf per year.</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -823,25 +823,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -854,42 +839,96 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,44 +938,8 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1372,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460CD49-F28E-4E8F-9EC7-325148866036}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G18"/>
+    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1382,7 +1385,7 @@
     <col min="2" max="2" width="14.453125" customWidth="1"/>
     <col min="3" max="3" width="8.1796875" customWidth="1"/>
     <col min="4" max="4" width="7.90625" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
     <col min="6" max="6" width="7.7265625" customWidth="1"/>
     <col min="7" max="7" width="7.1796875" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
@@ -1409,712 +1412,712 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="69" t="s">
+      <c r="I5" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="71"/>
+    </row>
+    <row r="6" spans="1:21" s="39" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="K5" s="69" t="s">
+      <c r="N6" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="L5" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="73"/>
-    </row>
-    <row r="6" spans="1:21" s="41" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="55" t="s">
+      <c r="O6" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="P6" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="N6" s="55" t="s">
+      <c r="Q6" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="O6" s="55" t="s">
+      <c r="R6" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="P6" s="55" t="s">
+      <c r="S6" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="Q6" s="56" t="s">
+      <c r="T6" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="56" t="s">
+      <c r="U6" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="S6" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="T6" s="56" t="s">
+    </row>
+    <row r="7" spans="1:21" s="39" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="68"/>
+      <c r="I7" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="U6" s="56" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="41" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="45"/>
-      <c r="I7" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="J7" s="57">
+      <c r="J7" s="49">
         <f>B13</f>
         <v>0</v>
       </c>
-      <c r="K7" s="58">
+      <c r="K7" s="50">
         <v>9</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L7" s="51">
         <v>2.8</v>
       </c>
-      <c r="M7" s="59">
+      <c r="M7" s="51">
         <v>0.3</v>
       </c>
-      <c r="N7" s="59">
+      <c r="N7" s="51">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O7" s="59">
+      <c r="O7" s="51">
         <v>1.5</v>
       </c>
-      <c r="P7" s="59">
+      <c r="P7" s="51">
         <f>SUM(L7:O7)</f>
         <v>9</v>
       </c>
-      <c r="Q7" s="60">
-        <f>L7/$K7</f>
+      <c r="Q7" s="52">
+        <f t="shared" ref="Q7:T11" si="0">L7/$K7</f>
         <v>0.31111111111111112</v>
       </c>
-      <c r="R7" s="60">
-        <f>M7/$K7</f>
+      <c r="R7" s="52">
+        <f t="shared" si="0"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="S7" s="60">
-        <f>N7/$K7</f>
+      <c r="S7" s="52">
+        <f t="shared" si="0"/>
         <v>0.48888888888888893</v>
       </c>
-      <c r="T7" s="60">
-        <f>O7/$K7</f>
+      <c r="T7" s="52">
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="U7" s="74">
+      <c r="U7" s="78">
         <f>SUM(Q7:T7)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B8" s="47">
-        <v>0</v>
-      </c>
-      <c r="C8" s="48">
-        <v>0</v>
-      </c>
-      <c r="D8" s="48">
-        <v>0</v>
-      </c>
-      <c r="E8" s="48">
-        <v>0</v>
-      </c>
-      <c r="F8" s="48">
-        <v>0</v>
-      </c>
-      <c r="G8" s="48">
+    <row r="8" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B8" s="42">
+        <v>0</v>
+      </c>
+      <c r="C8" s="43">
+        <v>0</v>
+      </c>
+      <c r="D8" s="43">
+        <v>0</v>
+      </c>
+      <c r="E8" s="43">
+        <v>0</v>
+      </c>
+      <c r="F8" s="43">
+        <v>0</v>
+      </c>
+      <c r="G8" s="43">
         <f>SUM(C8:F8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="J8" s="57">
+      <c r="I8" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" s="49">
         <f>B14</f>
         <v>0.3</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="53">
         <f>K$7-J8</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="L8" s="54">
-        <f>L$7-C14</f>
+      <c r="L8" s="46">
+        <f t="shared" ref="L8:O11" si="1">L$7-C14</f>
         <v>2.5599999999999996</v>
       </c>
-      <c r="M8" s="54">
-        <f>M$7-D14</f>
+      <c r="M8" s="46">
+        <f t="shared" si="1"/>
         <v>0.29000999999999999</v>
       </c>
-      <c r="N8" s="54">
-        <f>N$7-E14</f>
+      <c r="N8" s="46">
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="O8" s="54">
-        <f>O$7-F14</f>
+      <c r="O8" s="46">
+        <f t="shared" si="1"/>
         <v>1.4499900000000001</v>
       </c>
-      <c r="P8" s="59">
-        <f t="shared" ref="P8:P11" si="0">SUM(L8:O8)</f>
+      <c r="P8" s="51">
+        <f t="shared" ref="P8:P11" si="2">SUM(L8:O8)</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="Q8" s="60">
-        <f>L8/$K8</f>
+      <c r="Q8" s="52">
+        <f t="shared" si="0"/>
         <v>0.29425287356321839</v>
       </c>
-      <c r="R8" s="60">
-        <f>M8/$K8</f>
+      <c r="R8" s="52">
+        <f t="shared" si="0"/>
         <v>3.3334482758620693E-2</v>
       </c>
-      <c r="S8" s="60">
-        <f>N8/$K8</f>
+      <c r="S8" s="52">
+        <f t="shared" si="0"/>
         <v>0.50574712643678166</v>
       </c>
-      <c r="T8" s="60">
-        <f>O8/$K8</f>
+      <c r="T8" s="52">
+        <f t="shared" si="0"/>
         <v>0.16666551724137935</v>
       </c>
-      <c r="U8" s="74">
-        <f t="shared" ref="U8:U13" si="1">SUM(Q8:T8)</f>
+      <c r="U8" s="78">
+        <f t="shared" ref="U8:U13" si="3">SUM(Q8:T8)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B9" s="47" t="s">
+    <row r="9" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B9" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="44">
         <v>0.8</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="44">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E9" s="49">
-        <v>0</v>
-      </c>
-      <c r="F9" s="49">
+      <c r="E9" s="44">
+        <v>0</v>
+      </c>
+      <c r="F9" s="44">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G9" s="49">
-        <f t="shared" ref="G9:G10" si="2">SUM(C9:F9)</f>
+      <c r="G9" s="44">
+        <f t="shared" ref="G9:G10" si="4">SUM(C9:F9)</f>
         <v>1</v>
       </c>
-      <c r="I9" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="57">
+      <c r="I9" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="49">
         <f>B15</f>
         <v>0.4</v>
       </c>
-      <c r="K9" s="61">
+      <c r="K9" s="53">
         <f>K$7-J9</f>
         <v>8.6</v>
       </c>
-      <c r="L9" s="54">
-        <f>L$7-C15</f>
+      <c r="L9" s="46">
+        <f t="shared" si="1"/>
         <v>2.51667</v>
       </c>
-      <c r="M9" s="54">
-        <f>M$7-D15</f>
+      <c r="M9" s="46">
+        <f t="shared" si="1"/>
         <v>0.28667999999999999</v>
       </c>
-      <c r="N9" s="54">
-        <f>N$7-E15</f>
+      <c r="N9" s="46">
+        <f t="shared" si="1"/>
         <v>4.3633300000000004</v>
       </c>
-      <c r="O9" s="54">
-        <f>O$7-F15</f>
+      <c r="O9" s="46">
+        <f t="shared" si="1"/>
         <v>1.4333199999999999</v>
       </c>
-      <c r="P9" s="59">
+      <c r="P9" s="51">
+        <f t="shared" si="2"/>
+        <v>8.6</v>
+      </c>
+      <c r="Q9" s="52">
         <f t="shared" si="0"/>
-        <v>8.6</v>
-      </c>
-      <c r="Q9" s="60">
-        <f>L9/$K9</f>
         <v>0.29263604651162789</v>
       </c>
-      <c r="R9" s="60">
-        <f>M9/$K9</f>
+      <c r="R9" s="52">
+        <f t="shared" si="0"/>
         <v>3.3334883720930235E-2</v>
       </c>
-      <c r="S9" s="60">
-        <f>N9/$K9</f>
+      <c r="S9" s="52">
+        <f t="shared" si="0"/>
         <v>0.50736395348837215</v>
       </c>
-      <c r="T9" s="60">
-        <f>O9/$K9</f>
+      <c r="T9" s="52">
+        <f t="shared" si="0"/>
         <v>0.16666511627906977</v>
       </c>
-      <c r="U9" s="74">
-        <f t="shared" si="1"/>
+      <c r="U9" s="78">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+    <row r="10" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B10" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="44">
         <v>0.43330000000000002</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="44">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="44">
         <v>0.36670000000000003</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="44">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G10" s="49">
-        <f t="shared" si="2"/>
+      <c r="G10" s="44">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I10" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" s="57">
+      <c r="I10" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="49">
         <f>B16</f>
         <v>1</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="53">
         <f>K$7-J10</f>
         <v>8</v>
       </c>
-      <c r="L10" s="54">
-        <f>L$7-C16</f>
+      <c r="L10" s="46">
+        <f t="shared" si="1"/>
         <v>2.2566899999999999</v>
       </c>
-      <c r="M10" s="54">
-        <f>M$7-D16</f>
+      <c r="M10" s="46">
+        <f t="shared" si="1"/>
         <v>0.26669999999999999</v>
       </c>
-      <c r="N10" s="54">
-        <f>N$7-E16</f>
+      <c r="N10" s="46">
+        <f t="shared" si="1"/>
         <v>4.1433100000000005</v>
       </c>
-      <c r="O10" s="54">
-        <f>O$7-F16</f>
+      <c r="O10" s="46">
+        <f t="shared" si="1"/>
         <v>1.3332999999999999</v>
       </c>
-      <c r="P10" s="59">
+      <c r="P10" s="51">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q10" s="52">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q10" s="60">
-        <f>L10/$K10</f>
         <v>0.28208624999999998</v>
       </c>
-      <c r="R10" s="60">
-        <f>M10/$K10</f>
+      <c r="R10" s="52">
+        <f t="shared" si="0"/>
         <v>3.3337499999999999E-2</v>
       </c>
-      <c r="S10" s="60">
-        <f>N10/$K10</f>
+      <c r="S10" s="52">
+        <f t="shared" si="0"/>
         <v>0.51791375000000006</v>
       </c>
-      <c r="T10" s="60">
-        <f>O10/$K10</f>
+      <c r="T10" s="52">
+        <f t="shared" si="0"/>
         <v>0.16666249999999999</v>
       </c>
-      <c r="U10" s="74">
-        <f t="shared" si="1"/>
+      <c r="U10" s="78">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
+    <row r="11" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B11" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="I11" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11" s="57">
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="I11" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="49">
         <f>B17</f>
         <v>1.5</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="53">
         <f>K$7-J11</f>
         <v>7.5</v>
       </c>
-      <c r="L11" s="54">
-        <f>L$7-C17</f>
+      <c r="L11" s="46">
+        <f t="shared" si="1"/>
         <v>2.0400399999999999</v>
       </c>
-      <c r="M11" s="54">
-        <f>M$7-D17</f>
+      <c r="M11" s="46">
+        <f t="shared" si="1"/>
         <v>0.25004999999999999</v>
       </c>
-      <c r="N11" s="54">
-        <f>N$7-E17</f>
+      <c r="N11" s="46">
+        <f t="shared" si="1"/>
         <v>3.9599600000000001</v>
       </c>
-      <c r="O11" s="54">
-        <f>O$7-F17</f>
+      <c r="O11" s="46">
+        <f t="shared" si="1"/>
         <v>1.2499500000000001</v>
       </c>
-      <c r="P11" s="59">
+      <c r="P11" s="51">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="Q11" s="52">
         <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="Q11" s="60">
-        <f>L11/$K11</f>
         <v>0.27200533333333332</v>
       </c>
-      <c r="R11" s="60">
-        <f>M11/$K11</f>
+      <c r="R11" s="52">
+        <f t="shared" si="0"/>
         <v>3.3340000000000002E-2</v>
       </c>
-      <c r="S11" s="60">
-        <f>N11/$K11</f>
+      <c r="S11" s="52">
+        <f t="shared" si="0"/>
         <v>0.52799466666666672</v>
       </c>
-      <c r="T11" s="60">
-        <f>O11/$K11</f>
+      <c r="T11" s="52">
+        <f t="shared" si="0"/>
         <v>0.16666</v>
       </c>
-      <c r="U11" s="74">
-        <f t="shared" si="1"/>
+      <c r="U11" s="78">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="I12" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="J12" s="57" t="s">
+    <row r="12" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B12" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="I12" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="K12" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="L12" s="62" t="s">
+      <c r="K12" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="L12" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="62" t="s">
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="64"/>
-    </row>
-    <row r="13" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B13" s="47">
-        <v>0</v>
-      </c>
-      <c r="C13" s="53">
-        <v>0</v>
-      </c>
-      <c r="D13" s="53">
-        <v>0</v>
-      </c>
-      <c r="E13" s="53">
-        <v>0</v>
-      </c>
-      <c r="F13" s="53">
-        <v>0</v>
-      </c>
-      <c r="G13" s="53">
+      <c r="R12" s="76"/>
+      <c r="S12" s="76"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="77"/>
+    </row>
+    <row r="13" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B13" s="42">
+        <v>0</v>
+      </c>
+      <c r="C13" s="45">
+        <v>0</v>
+      </c>
+      <c r="D13" s="45">
+        <v>0</v>
+      </c>
+      <c r="E13" s="45">
+        <v>0</v>
+      </c>
+      <c r="F13" s="45">
+        <v>0</v>
+      </c>
+      <c r="G13" s="45">
         <f>SUM(C13:F13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="J13" s="57">
+      <c r="I13" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="49">
         <v>2.7</v>
       </c>
-      <c r="K13" s="61">
+      <c r="K13" s="53">
         <f>K$7-J13</f>
         <v>6.3</v>
       </c>
-      <c r="L13" s="54">
+      <c r="L13" s="46">
         <f>L11-C10*($K11-$K13)</f>
         <v>1.5200799999999997</v>
       </c>
-      <c r="M13" s="54">
+      <c r="M13" s="46">
         <f>M11-D10*($K11-$K13)</f>
         <v>0.21009</v>
       </c>
-      <c r="N13" s="54">
+      <c r="N13" s="46">
         <f>N11-E10*($K11-$K13)</f>
         <v>3.5199199999999999</v>
       </c>
-      <c r="O13" s="54">
+      <c r="O13" s="46">
         <f>O11-F10*($K11-$K13)</f>
         <v>1.0499100000000001</v>
       </c>
-      <c r="P13" s="54">
+      <c r="P13" s="46">
         <f>P11-G10*($K11-$K13)</f>
         <v>6.3</v>
       </c>
-      <c r="Q13" s="60">
+      <c r="Q13" s="52">
         <f>L13/$K13</f>
         <v>0.24128253968253963</v>
       </c>
-      <c r="R13" s="60">
+      <c r="R13" s="52">
         <f>M13/$K13</f>
         <v>3.334761904761905E-2</v>
       </c>
-      <c r="S13" s="60">
+      <c r="S13" s="52">
         <f>N13/$K13</f>
         <v>0.55871746031746028</v>
       </c>
-      <c r="T13" s="60">
+      <c r="T13" s="52">
         <f>O13/$K13</f>
         <v>0.16665238095238097</v>
       </c>
-      <c r="U13" s="74">
-        <f t="shared" si="1"/>
+      <c r="U13" s="58">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B14" s="47">
+    <row r="14" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B14" s="42">
         <v>0.3</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="46">
         <f>$B14*C9</f>
         <v>0.24</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="46">
         <f>$B14*D9</f>
         <v>9.9900000000000006E-3</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="46">
         <f>$B14*E9</f>
         <v>0</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="46">
         <f>$B14*F9</f>
         <v>5.0009999999999992E-2</v>
       </c>
-      <c r="G14" s="54">
+      <c r="G14" s="46">
         <f>SUM(C14:F14)</f>
         <v>0.3</v>
       </c>
-      <c r="I14" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="J14" s="68"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="66"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="75"/>
-    </row>
-    <row r="15" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B15" s="47">
+      <c r="I14" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="57"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="59"/>
+    </row>
+    <row r="15" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B15" s="42">
         <v>0.4</v>
       </c>
-      <c r="C15" s="54">
-        <f>C$14+C$10*($B15-$B$14)</f>
+      <c r="C15" s="46">
+        <f t="shared" ref="C15:F17" si="5">C$14+C$10*($B15-$B$14)</f>
         <v>0.28333000000000003</v>
       </c>
-      <c r="D15" s="54">
-        <f>D$14+D$10*($B15-$B$14)</f>
+      <c r="D15" s="46">
+        <f t="shared" si="5"/>
         <v>1.3320000000000002E-2</v>
       </c>
-      <c r="E15" s="54">
-        <f>E$14+E$10*($B15-$B$14)</f>
+      <c r="E15" s="46">
+        <f t="shared" si="5"/>
         <v>3.6670000000000015E-2</v>
       </c>
-      <c r="F15" s="54">
-        <f>F$14+F$10*($B15-$B$14)</f>
+      <c r="F15" s="46">
+        <f t="shared" si="5"/>
         <v>6.6679999999999989E-2</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="46">
         <f>SUM(C15:F15)</f>
         <v>0.4</v>
       </c>
-      <c r="I15" s="68" t="s">
-        <v>144</v>
-      </c>
-      <c r="J15" s="68"/>
-      <c r="U15" s="76"/>
-    </row>
-    <row r="16" spans="1:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B16" s="47">
+      <c r="I15" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" s="57"/>
+      <c r="U15" s="60"/>
+    </row>
+    <row r="16" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B16" s="42">
         <v>1</v>
       </c>
-      <c r="C16" s="54">
-        <f>C$14+C$10*($B16-$B$14)</f>
+      <c r="C16" s="46">
+        <f t="shared" si="5"/>
         <v>0.54330999999999996</v>
       </c>
-      <c r="D16" s="54">
-        <f>D$14+D$10*($B16-$B$14)</f>
+      <c r="D16" s="46">
+        <f t="shared" si="5"/>
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E16" s="54">
-        <f>E$14+E$10*($B16-$B$14)</f>
+      <c r="E16" s="46">
+        <f t="shared" si="5"/>
         <v>0.25669000000000003</v>
       </c>
-      <c r="F16" s="54">
-        <f>F$14+F$10*($B16-$B$14)</f>
+      <c r="F16" s="46">
+        <f t="shared" si="5"/>
         <v>0.16669999999999999</v>
       </c>
-      <c r="G16" s="54">
-        <f t="shared" ref="G16:G17" si="3">SUM(C16:F16)</f>
+      <c r="G16" s="46">
+        <f t="shared" ref="G16:G17" si="6">SUM(C16:F16)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="U16" s="76"/>
-    </row>
-    <row r="17" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B17" s="47">
+      <c r="U16" s="60"/>
+    </row>
+    <row r="17" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B17" s="42">
         <v>1.5</v>
       </c>
-      <c r="C17" s="54">
-        <f>C$14+C$10*($B17-$B$14)</f>
+      <c r="C17" s="46">
+        <f t="shared" si="5"/>
         <v>0.75995999999999997</v>
       </c>
-      <c r="D17" s="54">
-        <f>D$14+D$10*($B17-$B$14)</f>
+      <c r="D17" s="46">
+        <f t="shared" si="5"/>
         <v>4.9950000000000001E-2</v>
       </c>
-      <c r="E17" s="54">
-        <f>E$14+E$10*($B17-$B$14)</f>
+      <c r="E17" s="46">
+        <f t="shared" si="5"/>
         <v>0.44004000000000004</v>
       </c>
-      <c r="F17" s="54">
-        <f>F$14+F$10*($B17-$B$14)</f>
+      <c r="F17" s="46">
+        <f t="shared" si="5"/>
         <v>0.25004999999999994</v>
       </c>
-      <c r="G17" s="54">
-        <f t="shared" si="3"/>
+      <c r="G17" s="46">
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
-      <c r="U17" s="76"/>
-    </row>
-    <row r="18" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="s">
+      <c r="U17" s="60"/>
+    </row>
+    <row r="18" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B18" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="U18" s="76"/>
-    </row>
-    <row r="19" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U19" s="76"/>
-    </row>
-    <row r="20" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U20" s="76"/>
-    </row>
-    <row r="21" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U21" s="76"/>
-    </row>
-    <row r="22" spans="2:21" s="46" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="U22" s="76"/>
-    </row>
-    <row r="23" spans="2:21" s="46" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="U23" s="76"/>
-    </row>
-    <row r="24" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U24" s="76"/>
-    </row>
-    <row r="25" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U25" s="76"/>
-    </row>
-    <row r="26" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U26" s="76"/>
-    </row>
-    <row r="27" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U27" s="76"/>
-    </row>
-    <row r="28" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U28" s="76"/>
-    </row>
-    <row r="29" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U29" s="76"/>
-    </row>
-    <row r="30" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U30" s="76"/>
-    </row>
-    <row r="31" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U31" s="76"/>
-    </row>
-    <row r="32" spans="2:21" s="46" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="U32" s="76"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="U18" s="60"/>
+    </row>
+    <row r="19" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U19" s="60"/>
+    </row>
+    <row r="20" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U20" s="60"/>
+    </row>
+    <row r="21" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U21" s="60"/>
+    </row>
+    <row r="22" spans="2:21" s="41" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U22" s="60"/>
+    </row>
+    <row r="23" spans="2:21" s="41" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="60"/>
+    </row>
+    <row r="24" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U24" s="60"/>
+    </row>
+    <row r="25" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U25" s="60"/>
+    </row>
+    <row r="26" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U26" s="60"/>
+    </row>
+    <row r="27" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U27" s="60"/>
+    </row>
+    <row r="28" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U28" s="60"/>
+    </row>
+    <row r="29" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U29" s="60"/>
+    </row>
+    <row r="30" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U30" s="60"/>
+    </row>
+    <row r="31" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U31" s="60"/>
+    </row>
+    <row r="32" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="U32" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="L12:P12"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="L12:P12"/>
-    <mergeCell ref="Q12:U12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4304,14 +4307,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -4407,10 +4410,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>
@@ -4515,10 +4518,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Add recent water consumption to model guide file from water use reports
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840615DB-7AD2-4B80-8DEA-B59C885C4C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB4D5D6-C63E-481B-8B5E-5F1401AC5F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="151">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -515,19 +515,13 @@
     <t>** If percentage shares of total shortages for 0.3 to 1.5 maf per year are continue to total shortages for 1.5 to 2.7 maf per year.</t>
   </si>
   <si>
-    <t>Lake Mead withdraws (Consumptive</t>
-  </si>
-  <si>
     <t>Recent Lake Mead Withdraws (Consumptive Use)</t>
   </si>
   <si>
-    <t>Recent Lake Mead Withdraws are calculated as the user's historical allocation minus their water conservation account deposit</t>
-  </si>
-  <si>
     <t>Withdraws</t>
   </si>
   <si>
-    <t>Recent Lake Mead user withdrawals calculated as historical allocation minus Water Conservation Account credit.</t>
+    <t>Recent Lake Mead user withdrawals reported in water accounting reports</t>
   </si>
 </sst>
 </file>
@@ -751,7 +745,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -912,6 +906,15 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -959,12 +962,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1250,9 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1330,10 +1325,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1756,29 +1751,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="77" t="s">
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="80" t="s">
         <v>146</v>
       </c>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="79"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="82"/>
     </row>
     <row r="6" spans="1:21" s="39" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="40" t="s">
@@ -1799,9 +1794,9 @@
       <c r="G6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
       <c r="L6" s="47" t="s">
         <v>128</v>
       </c>
@@ -1834,14 +1829,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="39" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="71"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
       <c r="I7" s="49" t="s">
         <v>139</v>
       </c>
@@ -2109,13 +2104,13 @@
       <c r="B11" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
       <c r="I11" s="49" t="s">
         <v>125</v>
       </c>
@@ -2169,14 +2164,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
       <c r="I12" s="49" t="s">
         <v>126</v>
       </c>
@@ -2186,20 +2181,20 @@
       <c r="K12" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="L12" s="66" t="s">
+      <c r="L12" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="66" t="s">
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="R12" s="67"/>
-      <c r="S12" s="67"/>
-      <c r="T12" s="67"/>
-      <c r="U12" s="68"/>
+      <c r="R12" s="70"/>
+      <c r="S12" s="70"/>
+      <c r="T12" s="70"/>
+      <c r="U12" s="71"/>
     </row>
     <row r="13" spans="1:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="42">
@@ -2398,13 +2393,13 @@
       <c r="B18" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
       <c r="U18" s="60"/>
     </row>
     <row r="19" spans="2:21" s="41" customFormat="1" ht="14" x14ac:dyDescent="0.3">
@@ -4458,10 +4453,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23193A-BD0C-4DE4-9C7D-76BA13A71C88}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F15"/>
+      <selection activeCell="A4" sqref="A4:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4469,298 +4464,244 @@
     <col min="1" max="1" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="12">
-        <f>SUM(C5:F5)</f>
-        <v>9</v>
-      </c>
-      <c r="C5" s="12">
-        <v>2.8</v>
-      </c>
-      <c r="D5" s="12">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="80" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="64" t="str">
         <f>Deposits!A1</f>
         <v>Year</v>
       </c>
-      <c r="B6" s="80" t="str">
-        <f>Deposits!B1</f>
-        <v>Total</v>
-      </c>
-      <c r="C6" s="80" t="str">
+      <c r="B4" s="64" t="str">
         <f>Deposits!C1</f>
         <v>Arizona</v>
       </c>
-      <c r="D6" s="80" t="str">
+      <c r="C4" s="64" t="str">
         <f>Deposits!D1</f>
         <v>California</v>
       </c>
-      <c r="E6" s="80" t="str">
+      <c r="D4" s="64" t="str">
         <f>Deposits!E1</f>
         <v>Nevada</v>
       </c>
-      <c r="F6" s="80" t="str">
+      <c r="E4" s="64" t="str">
         <f>Deposits!F1</f>
         <v>Mexico</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F4" s="64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="62">
+        <f>Deposits!A18</f>
+        <v>2023</v>
+      </c>
+      <c r="B5" s="65">
+        <v>1.89</v>
+      </c>
+      <c r="C5" s="65">
+        <v>3.6989999999999998</v>
+      </c>
+      <c r="D5" s="65">
+        <v>0.187</v>
+      </c>
+      <c r="E5" s="65">
+        <v>1.43</v>
+      </c>
+      <c r="F5" s="66">
+        <f>SUM(B5:E5)</f>
+        <v>7.2059999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="62">
+        <f>Deposits!A17</f>
+        <v>2022</v>
+      </c>
+      <c r="B6" s="65">
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="C6" s="65">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="D6" s="65">
+        <v>0.224</v>
+      </c>
+      <c r="E6" s="65">
+        <v>1.45</v>
+      </c>
+      <c r="F6" s="66">
+        <f t="shared" ref="F6:F13" si="0">SUM(B6:E6)</f>
+        <v>8.1120000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
-        <f>Deposits!A10</f>
-        <v>2015</v>
-      </c>
-      <c r="B7" s="81">
-        <f>B$5-Deposits!B10/1000000</f>
-        <v>9.1250359999999997</v>
-      </c>
-      <c r="C7" s="81">
-        <f>C$5-Deposits!C10/1000000</f>
-        <v>2.8</v>
-      </c>
-      <c r="D7" s="81">
-        <f>D$5-Deposits!D10/1000000</f>
-        <v>4.4712940000000003</v>
-      </c>
-      <c r="E7" s="81">
-        <f>E$5-Deposits!E10/1000000</f>
-        <v>0.353742</v>
-      </c>
-      <c r="F7" s="81">
-        <f>F$5-Deposits!F10/1000000</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <f>Deposits!A16</f>
+        <v>2021</v>
+      </c>
+      <c r="B7" s="65">
+        <v>2.4260000000000002</v>
+      </c>
+      <c r="C7" s="65">
+        <v>4.4050000000000002</v>
+      </c>
+      <c r="D7" s="65">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="E7" s="65">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="F7" s="66">
+        <f t="shared" si="0"/>
+        <v>8.5280000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
-        <f>Deposits!A11</f>
-        <v>2016</v>
-      </c>
-      <c r="B8" s="81">
-        <f>B$5-Deposits!B11/1000000</f>
-        <v>8.9621860000000009</v>
-      </c>
-      <c r="C8" s="81">
-        <f>C$5-Deposits!C11/1000000</f>
-        <v>2.8</v>
-      </c>
-      <c r="D8" s="81">
-        <f>D$5-Deposits!D11/1000000</f>
-        <v>4.3827250000000006</v>
-      </c>
-      <c r="E8" s="81">
-        <f>E$5-Deposits!E11/1000000</f>
-        <v>0.27946099999999996</v>
-      </c>
-      <c r="F8" s="81">
-        <f>F$5-Deposits!F11/1000000</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <f>Deposits!A15</f>
+        <v>2020</v>
+      </c>
+      <c r="B8" s="65">
+        <v>2.4710000000000001</v>
+      </c>
+      <c r="C8" s="65">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D8" s="65">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E8" s="65">
+        <v>1.4319999999999999</v>
+      </c>
+      <c r="F8" s="66">
+        <f t="shared" si="0"/>
+        <v>8.2189999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
-        <f>Deposits!A12</f>
-        <v>2017</v>
-      </c>
-      <c r="B9" s="81">
-        <f>B$5-Deposits!B12/1000000</f>
-        <v>8.4881869999999999</v>
-      </c>
-      <c r="C9" s="81">
-        <f>C$5-Deposits!C12/1000000</f>
-        <v>2.7762499999999997</v>
-      </c>
-      <c r="D9" s="81">
-        <f>D$5-Deposits!D12/1000000</f>
-        <v>3.9626880000000004</v>
-      </c>
-      <c r="E9" s="81">
-        <f>E$5-Deposits!E12/1000000</f>
-        <v>0.249249</v>
-      </c>
-      <c r="F9" s="81">
-        <f>F$5-Deposits!F12/1000000</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <f>Deposits!A14</f>
+        <v>2019</v>
+      </c>
+      <c r="B9" s="65">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C9" s="65">
+        <v>3.84</v>
+      </c>
+      <c r="D9" s="65">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E9" s="65">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="F9" s="66">
+        <f t="shared" si="0"/>
+        <v>8.027000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="62">
         <f>Deposits!A13</f>
         <v>2018</v>
       </c>
-      <c r="B10" s="81">
-        <f>B$5-Deposits!B13/1000000</f>
-        <v>8.5195589999999992</v>
-      </c>
-      <c r="C10" s="81">
-        <f>C$5-Deposits!C13/1000000</f>
-        <v>2.5837479999999999</v>
-      </c>
-      <c r="D10" s="81">
-        <f>D$5-Deposits!D13/1000000</f>
-        <v>4.253946</v>
-      </c>
-      <c r="E10" s="81">
-        <f>E$5-Deposits!E13/1000000</f>
-        <v>0.181865</v>
-      </c>
-      <c r="F10" s="81">
-        <f>F$5-Deposits!F13/1000000</f>
+      <c r="B10" s="65">
+        <v>2.63</v>
+      </c>
+      <c r="C10" s="65">
+        <v>4.2</v>
+      </c>
+      <c r="D10" s="65">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="E10" s="65">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="F10" s="66">
+        <f t="shared" si="0"/>
+        <v>8.5670000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="62">
+        <f>Deposits!A12</f>
+        <v>2017</v>
+      </c>
+      <c r="B11" s="65">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C11" s="65">
+        <v>4.03</v>
+      </c>
+      <c r="D11" s="65">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E11" s="65">
+        <v>1.52</v>
+      </c>
+      <c r="F11" s="66">
+        <f t="shared" si="0"/>
+        <v>8.3030000000000008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="62">
+        <f>Deposits!A11</f>
+        <v>2016</v>
+      </c>
+      <c r="B12" s="65">
+        <v>2.61</v>
+      </c>
+      <c r="C12" s="65">
+        <v>4.38</v>
+      </c>
+      <c r="D12" s="65">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="E12" s="65">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="62">
-        <f>Deposits!A14</f>
-        <v>2019</v>
-      </c>
-      <c r="B11" s="81">
-        <f>B$5-Deposits!B14/1000000</f>
-        <v>8.2963299999999993</v>
-      </c>
-      <c r="C11" s="81">
-        <f>C$5-Deposits!C14/1000000</f>
-        <v>2.6695479999999998</v>
-      </c>
-      <c r="D11" s="81">
-        <f>D$5-Deposits!D14/1000000</f>
-        <v>4.0452220000000008</v>
-      </c>
-      <c r="E11" s="81">
-        <f>E$5-Deposits!E14/1000000</f>
-        <v>0.21453499999999998</v>
-      </c>
-      <c r="F11" s="81">
-        <f>F$5-Deposits!F14/1000000</f>
-        <v>1.3670249999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="62">
-        <f>Deposits!A15</f>
-        <v>2020</v>
-      </c>
-      <c r="B12" s="81">
-        <f>B$5-Deposits!B15/1000000</f>
-        <v>8.4312730000000009</v>
-      </c>
-      <c r="C12" s="81">
-        <f>C$5-Deposits!C15/1000000</f>
-        <v>2.6747619999999999</v>
-      </c>
-      <c r="D12" s="81">
-        <f>D$5-Deposits!D15/1000000</f>
-        <v>4.0773390000000003</v>
-      </c>
-      <c r="E12" s="81">
-        <f>E$5-Deposits!E15/1000000</f>
-        <v>0.22017199999999998</v>
-      </c>
-      <c r="F12" s="81">
-        <f>F$5-Deposits!F15/1000000</f>
-        <v>1.4590000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F12" s="66">
+        <f t="shared" si="0"/>
+        <v>8.7279999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
-        <f>Deposits!A16</f>
-        <v>2021</v>
-      </c>
-      <c r="B13" s="81">
-        <f>B$5-Deposits!B16/1000000</f>
-        <v>8.8084100000000003</v>
-      </c>
-      <c r="C13" s="81">
-        <f>C$5-Deposits!C16/1000000</f>
-        <v>2.7145409999999996</v>
-      </c>
-      <c r="D13" s="81">
-        <f>D$5-Deposits!D16/1000000</f>
-        <v>4.4187860000000008</v>
-      </c>
-      <c r="E13" s="81">
-        <f>E$5-Deposits!E16/1000000</f>
-        <v>0.21608299999999997</v>
-      </c>
-      <c r="F13" s="81">
-        <f>F$5-Deposits!F16/1000000</f>
-        <v>1.4590000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="62">
-        <f>Deposits!A17</f>
-        <v>2022</v>
-      </c>
-      <c r="B14" s="81">
-        <f>B$5-Deposits!B17/1000000</f>
-        <v>8.9230630000000009</v>
-      </c>
-      <c r="C14" s="81">
-        <f>C$5-Deposits!C17/1000000</f>
-        <v>2.7307779999999999</v>
-      </c>
-      <c r="D14" s="81">
-        <f>D$5-Deposits!D17/1000000</f>
-        <v>4.5113920000000007</v>
-      </c>
-      <c r="E14" s="81">
-        <f>E$5-Deposits!E17/1000000</f>
-        <v>0.210893</v>
-      </c>
-      <c r="F14" s="81">
-        <f>F$5-Deposits!F17/1000000</f>
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="62">
-        <f>Deposits!A18</f>
-        <v>2023</v>
-      </c>
-      <c r="B15" s="81">
-        <f>B$5-Deposits!B18/1000000</f>
-        <v>8.7439169999999997</v>
-      </c>
-      <c r="C15" s="81">
-        <f>C$5-Deposits!C18/1000000</f>
-        <v>2.8428339999999999</v>
-      </c>
-      <c r="D15" s="81">
-        <f>D$5-Deposits!D18/1000000</f>
-        <v>3.9838610000000005</v>
-      </c>
-      <c r="E15" s="81">
-        <f>E$5-Deposits!E18/1000000</f>
-        <v>0.38322200000000001</v>
-      </c>
-      <c r="F15" s="81">
-        <f>F$5-Deposits!F18/1000000</f>
-        <v>1.534</v>
+        <f>Deposits!A10</f>
+        <v>2015</v>
+      </c>
+      <c r="B13" s="65">
+        <v>2.6</v>
+      </c>
+      <c r="C13" s="65">
+        <v>4.62</v>
+      </c>
+      <c r="D13" s="65">
+        <v>0.223</v>
+      </c>
+      <c r="E13" s="65">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="66">
+        <f t="shared" si="0"/>
+        <v>8.9430000000000014</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E13">
+    <sortCondition descending="1" ref="A4:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4960,14 +4901,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -5063,10 +5004,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="65"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>
@@ -5171,10 +5112,10 @@
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="65"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="25" t="s">
         <v>63</v>
       </c>

</xml_diff>